<commit_message>
get 6m data, and draw chart of avg, based on open_percent.
</commit_message>
<xml_diff>
--- a/StockSmart/price.xlsx
+++ b/StockSmart/price.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="4" r:id="rId1"/>
@@ -14,9 +14,9 @@
   </sheets>
   <definedNames>
     <definedName name="_600036_12m" localSheetId="0">data!$A$1:$D$234</definedName>
+    <definedName name="_600036_data1" localSheetId="2">Sheet2!$H$28:$Q$52</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -32,11 +32,27 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="2" name="600036_data1" type="6" refreshedVersion="3" background="1" saveData="1">
+    <textPr codePage="936" sourceFile="D:\github\apps\StockSmart\600036_data1.txt" space="1" consecutive="1">
+      <textFields count="10">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="9">
   <si>
     <t>e</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -52,6 +68,21 @@
   <si>
     <t>min%</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>checking</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>avg</t>
   </si>
 </sst>
 </file>
@@ -103,7 +134,7 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -132,9 +163,9 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>data!$B:$B</c:f>
+              <c:f>data!$F:$F</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0_ </c:formatCode>
                 <c:ptCount val="1048576"/>
                 <c:pt idx="0">
                   <c:v>0.34310000000000002</c:v>
@@ -1553,11 +1584,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="77783808"/>
-        <c:axId val="77786112"/>
+        <c:axId val="65897600"/>
+        <c:axId val="65899904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77783808"/>
+        <c:axId val="65897600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1567,14 +1598,14 @@
         <c:title>
           <c:layout/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0_ " sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77786112"/>
+        <c:crossAx val="65899904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="77786112"/>
+        <c:axId val="65899904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1589,8 +1620,440 @@
         <c:spPr>
           <a:ln w="6350"/>
         </c:spPr>
-        <c:crossAx val="77783808"/>
+        <c:crossAx val="65897600"/>
         <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="zh-CN"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>count</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$I$28:$I$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>-2.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$K$28:$K$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="37016320"/>
+        <c:axId val="37548800"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>avg</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$I$28:$I$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>-2.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$Q$28:$Q$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.2200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.68</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.18888888889</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.5315789473700001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.4249999999999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.4750000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.55</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.5571428571400001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.5499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="112002560"/>
+        <c:axId val="111854336"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="37016320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="37548800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="37548800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="37016320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="111854336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="112002560"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="112002560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="111854336"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
@@ -1605,6 +2068,7 @@
     <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId1"/>
 </c:chartSpace>
 </file>
 
@@ -1640,15 +2104,90 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="图表 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.12794</cdr:x>
+      <cdr:y>0.1128</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.26407</cdr:x>
+      <cdr:y>0.21692</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1190625" y="495300"/>
+          <a:ext cx="1266825" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>60036 6m</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="600036_12m" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="600036_data1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1934,8 +2473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N234"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -5945,8 +6484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="P53" sqref="P53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -5965,14 +6504,823 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="H28:Q52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
+  <cols>
+    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5" customWidth="1"/>
+    <col min="10" max="10" width="6.5" customWidth="1"/>
+    <col min="11" max="11" width="3.5" customWidth="1"/>
+    <col min="12" max="16" width="4.5" customWidth="1"/>
+    <col min="17" max="17" width="12.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="28" spans="8:17">
+      <c r="H28" t="s">
+        <v>4</v>
+      </c>
+      <c r="I28">
+        <v>-2.9</v>
+      </c>
+      <c r="J28" t="s">
+        <v>5</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28" t="s">
+        <v>6</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28" t="s">
+        <v>7</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="8:17">
+      <c r="H29" t="s">
+        <v>4</v>
+      </c>
+      <c r="I29">
+        <v>-2.7</v>
+      </c>
+      <c r="J29" t="s">
+        <v>5</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29" t="s">
+        <v>6</v>
+      </c>
+      <c r="M29">
+        <v>2</v>
+      </c>
+      <c r="N29" t="s">
+        <v>7</v>
+      </c>
+      <c r="O29">
+        <v>2</v>
+      </c>
+      <c r="P29" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="8:17">
+      <c r="H30" t="s">
+        <v>4</v>
+      </c>
+      <c r="I30">
+        <v>-1.7</v>
+      </c>
+      <c r="J30" t="s">
+        <v>5</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30" t="s">
+        <v>6</v>
+      </c>
+      <c r="M30">
+        <v>1.2</v>
+      </c>
+      <c r="N30" t="s">
+        <v>7</v>
+      </c>
+      <c r="O30">
+        <v>1.2</v>
+      </c>
+      <c r="P30" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q30">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="31" spans="8:17">
+      <c r="H31" t="s">
+        <v>4</v>
+      </c>
+      <c r="I31">
+        <v>-1.3</v>
+      </c>
+      <c r="J31" t="s">
+        <v>5</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31" t="s">
+        <v>6</v>
+      </c>
+      <c r="M31">
+        <v>0.1</v>
+      </c>
+      <c r="N31" t="s">
+        <v>7</v>
+      </c>
+      <c r="O31">
+        <v>0.1</v>
+      </c>
+      <c r="P31" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q31">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="32" spans="8:17">
+      <c r="H32" t="s">
+        <v>4</v>
+      </c>
+      <c r="I32">
+        <v>-1.2</v>
+      </c>
+      <c r="J32" t="s">
+        <v>5</v>
+      </c>
+      <c r="K32">
+        <v>2</v>
+      </c>
+      <c r="L32" t="s">
+        <v>6</v>
+      </c>
+      <c r="M32">
+        <v>3</v>
+      </c>
+      <c r="N32" t="s">
+        <v>7</v>
+      </c>
+      <c r="O32">
+        <v>1</v>
+      </c>
+      <c r="P32" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="8:17">
+      <c r="H33" t="s">
+        <v>4</v>
+      </c>
+      <c r="I33">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="J33" t="s">
+        <v>5</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="L33" t="s">
+        <v>6</v>
+      </c>
+      <c r="M33">
+        <v>1</v>
+      </c>
+      <c r="N33" t="s">
+        <v>7</v>
+      </c>
+      <c r="O33">
+        <v>1</v>
+      </c>
+      <c r="P33" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="8:17">
+      <c r="H34" t="s">
+        <v>4</v>
+      </c>
+      <c r="I34">
+        <v>-1</v>
+      </c>
+      <c r="J34" t="s">
+        <v>5</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34" t="s">
+        <v>6</v>
+      </c>
+      <c r="M34">
+        <v>1.2</v>
+      </c>
+      <c r="N34" t="s">
+        <v>7</v>
+      </c>
+      <c r="O34">
+        <v>1.2</v>
+      </c>
+      <c r="P34" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q34">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="35" spans="8:17">
+      <c r="H35" t="s">
+        <v>4</v>
+      </c>
+      <c r="I35">
+        <v>-0.9</v>
+      </c>
+      <c r="J35" t="s">
+        <v>5</v>
+      </c>
+      <c r="K35">
+        <v>2</v>
+      </c>
+      <c r="L35" t="s">
+        <v>6</v>
+      </c>
+      <c r="M35">
+        <v>2.1</v>
+      </c>
+      <c r="N35" t="s">
+        <v>7</v>
+      </c>
+      <c r="O35">
+        <v>0.2</v>
+      </c>
+      <c r="P35" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q35">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="8:17">
+      <c r="H36" t="s">
+        <v>4</v>
+      </c>
+      <c r="I36">
+        <v>-0.8</v>
+      </c>
+      <c r="J36" t="s">
+        <v>5</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36" t="s">
+        <v>6</v>
+      </c>
+      <c r="M36">
+        <v>6.1</v>
+      </c>
+      <c r="N36" t="s">
+        <v>7</v>
+      </c>
+      <c r="O36">
+        <v>6.1</v>
+      </c>
+      <c r="P36" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q36">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="37" spans="8:17">
+      <c r="H37" t="s">
+        <v>4</v>
+      </c>
+      <c r="I37">
+        <v>-0.7</v>
+      </c>
+      <c r="J37" t="s">
+        <v>5</v>
+      </c>
+      <c r="K37">
+        <v>5</v>
+      </c>
+      <c r="L37" t="s">
+        <v>6</v>
+      </c>
+      <c r="M37">
+        <v>4.5</v>
+      </c>
+      <c r="N37" t="s">
+        <v>7</v>
+      </c>
+      <c r="O37">
+        <v>0.9</v>
+      </c>
+      <c r="P37" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q37">
+        <v>2.2200000000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="8:17">
+      <c r="H38" t="s">
+        <v>4</v>
+      </c>
+      <c r="I38">
+        <v>-0.6</v>
+      </c>
+      <c r="J38" t="s">
+        <v>5</v>
+      </c>
+      <c r="K38">
+        <v>2</v>
+      </c>
+      <c r="L38" t="s">
+        <v>6</v>
+      </c>
+      <c r="M38">
+        <v>0.4</v>
+      </c>
+      <c r="N38" t="s">
+        <v>7</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q38">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="39" spans="8:17">
+      <c r="H39" t="s">
+        <v>4</v>
+      </c>
+      <c r="I39">
+        <v>-0.5</v>
+      </c>
+      <c r="J39" t="s">
+        <v>5</v>
+      </c>
+      <c r="K39">
+        <v>3</v>
+      </c>
+      <c r="L39" t="s">
+        <v>6</v>
+      </c>
+      <c r="M39">
+        <v>0.9</v>
+      </c>
+      <c r="N39" t="s">
+        <v>7</v>
+      </c>
+      <c r="O39">
+        <v>0.4</v>
+      </c>
+      <c r="P39" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q39">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="40" spans="8:17">
+      <c r="H40" t="s">
+        <v>4</v>
+      </c>
+      <c r="I40">
+        <v>-0.4</v>
+      </c>
+      <c r="J40" t="s">
+        <v>5</v>
+      </c>
+      <c r="K40">
+        <v>4</v>
+      </c>
+      <c r="L40" t="s">
+        <v>6</v>
+      </c>
+      <c r="M40">
+        <v>1.6</v>
+      </c>
+      <c r="N40" t="s">
+        <v>7</v>
+      </c>
+      <c r="O40">
+        <v>0.1</v>
+      </c>
+      <c r="P40" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q40">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="41" spans="8:17">
+      <c r="H41" t="s">
+        <v>4</v>
+      </c>
+      <c r="I41">
+        <v>-0.3</v>
+      </c>
+      <c r="J41" t="s">
+        <v>5</v>
+      </c>
+      <c r="K41">
+        <v>5</v>
+      </c>
+      <c r="L41" t="s">
+        <v>6</v>
+      </c>
+      <c r="M41">
+        <v>6</v>
+      </c>
+      <c r="N41" t="s">
+        <v>7</v>
+      </c>
+      <c r="O41">
+        <v>0.5</v>
+      </c>
+      <c r="P41" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q41">
+        <v>2.68</v>
+      </c>
+    </row>
+    <row r="42" spans="8:17">
+      <c r="H42" t="s">
+        <v>4</v>
+      </c>
+      <c r="I42">
+        <v>-0.2</v>
+      </c>
+      <c r="J42" t="s">
+        <v>5</v>
+      </c>
+      <c r="K42">
+        <v>9</v>
+      </c>
+      <c r="L42" t="s">
+        <v>6</v>
+      </c>
+      <c r="M42">
+        <v>2.4</v>
+      </c>
+      <c r="N42" t="s">
+        <v>7</v>
+      </c>
+      <c r="O42">
+        <v>0.2</v>
+      </c>
+      <c r="P42" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q42">
+        <v>1.18888888889</v>
+      </c>
+    </row>
+    <row r="43" spans="8:17">
+      <c r="H43" t="s">
+        <v>4</v>
+      </c>
+      <c r="I43">
+        <v>-0.1</v>
+      </c>
+      <c r="J43" t="s">
+        <v>5</v>
+      </c>
+      <c r="K43">
+        <v>10</v>
+      </c>
+      <c r="L43" t="s">
+        <v>6</v>
+      </c>
+      <c r="M43">
+        <v>3.7</v>
+      </c>
+      <c r="N43" t="s">
+        <v>7</v>
+      </c>
+      <c r="O43">
+        <v>0.1</v>
+      </c>
+      <c r="P43" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q43">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="44" spans="8:17">
+      <c r="H44" t="s">
+        <v>4</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44" t="s">
+        <v>5</v>
+      </c>
+      <c r="K44">
+        <v>19</v>
+      </c>
+      <c r="L44" t="s">
+        <v>6</v>
+      </c>
+      <c r="M44">
+        <v>6.5</v>
+      </c>
+      <c r="N44" t="s">
+        <v>7</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+      <c r="P44" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q44">
+        <v>1.5315789473700001</v>
+      </c>
+    </row>
+    <row r="45" spans="8:17">
+      <c r="H45" t="s">
+        <v>4</v>
+      </c>
+      <c r="I45">
+        <v>0.1</v>
+      </c>
+      <c r="J45" t="s">
+        <v>5</v>
+      </c>
+      <c r="K45">
+        <v>8</v>
+      </c>
+      <c r="L45" t="s">
+        <v>6</v>
+      </c>
+      <c r="M45">
+        <v>4.3</v>
+      </c>
+      <c r="N45" t="s">
+        <v>7</v>
+      </c>
+      <c r="O45">
+        <v>0.1</v>
+      </c>
+      <c r="P45" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q45">
+        <v>2.4249999999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="8:17">
+      <c r="H46" t="s">
+        <v>4</v>
+      </c>
+      <c r="I46">
+        <v>0.2</v>
+      </c>
+      <c r="J46" t="s">
+        <v>5</v>
+      </c>
+      <c r="K46">
+        <v>8</v>
+      </c>
+      <c r="L46" t="s">
+        <v>6</v>
+      </c>
+      <c r="M46">
+        <v>6.2</v>
+      </c>
+      <c r="N46" t="s">
+        <v>7</v>
+      </c>
+      <c r="O46">
+        <v>0.3</v>
+      </c>
+      <c r="P46" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q46">
+        <v>2.4750000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="8:17">
+      <c r="H47" t="s">
+        <v>4</v>
+      </c>
+      <c r="I47">
+        <v>0.3</v>
+      </c>
+      <c r="J47" t="s">
+        <v>5</v>
+      </c>
+      <c r="K47">
+        <v>4</v>
+      </c>
+      <c r="L47" t="s">
+        <v>6</v>
+      </c>
+      <c r="M47">
+        <v>3</v>
+      </c>
+      <c r="N47" t="s">
+        <v>7</v>
+      </c>
+      <c r="O47">
+        <v>0.3</v>
+      </c>
+      <c r="P47" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q47">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="48" spans="8:17">
+      <c r="H48" t="s">
+        <v>4</v>
+      </c>
+      <c r="I48">
+        <v>0.4</v>
+      </c>
+      <c r="J48" t="s">
+        <v>5</v>
+      </c>
+      <c r="K48">
+        <v>7</v>
+      </c>
+      <c r="L48" t="s">
+        <v>6</v>
+      </c>
+      <c r="M48">
+        <v>5.2</v>
+      </c>
+      <c r="N48" t="s">
+        <v>7</v>
+      </c>
+      <c r="O48">
+        <v>1.3</v>
+      </c>
+      <c r="P48" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q48">
+        <v>2.5571428571400001</v>
+      </c>
+    </row>
+    <row r="49" spans="8:17">
+      <c r="H49" t="s">
+        <v>4</v>
+      </c>
+      <c r="I49">
+        <v>0.5</v>
+      </c>
+      <c r="J49" t="s">
+        <v>5</v>
+      </c>
+      <c r="K49">
+        <v>12</v>
+      </c>
+      <c r="L49" t="s">
+        <v>6</v>
+      </c>
+      <c r="M49">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="N49" t="s">
+        <v>7</v>
+      </c>
+      <c r="O49">
+        <v>0</v>
+      </c>
+      <c r="P49" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q49">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="50" spans="8:17">
+      <c r="H50" t="s">
+        <v>4</v>
+      </c>
+      <c r="I50">
+        <v>0.6</v>
+      </c>
+      <c r="J50" t="s">
+        <v>5</v>
+      </c>
+      <c r="K50">
+        <v>6</v>
+      </c>
+      <c r="L50" t="s">
+        <v>6</v>
+      </c>
+      <c r="M50">
+        <v>7.5</v>
+      </c>
+      <c r="N50" t="s">
+        <v>7</v>
+      </c>
+      <c r="O50">
+        <v>0.7</v>
+      </c>
+      <c r="P50" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q50">
+        <v>2.5499999999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="8:17">
+      <c r="H51" t="s">
+        <v>4</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="J51" t="s">
+        <v>5</v>
+      </c>
+      <c r="K51">
+        <v>1</v>
+      </c>
+      <c r="L51" t="s">
+        <v>6</v>
+      </c>
+      <c r="M51">
+        <v>0.6</v>
+      </c>
+      <c r="N51" t="s">
+        <v>7</v>
+      </c>
+      <c r="O51">
+        <v>0.6</v>
+      </c>
+      <c r="P51" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q51">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="52" spans="8:17">
+      <c r="H52" t="s">
+        <v>4</v>
+      </c>
+      <c r="I52">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J52" t="s">
+        <v>5</v>
+      </c>
+      <c r="K52">
+        <v>1</v>
+      </c>
+      <c r="L52" t="s">
+        <v>6</v>
+      </c>
+      <c r="M52">
+        <v>1</v>
+      </c>
+      <c r="N52" t="s">
+        <v>7</v>
+      </c>
+      <c r="O52">
+        <v>1</v>
+      </c>
+      <c r="P52" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q52">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
analyse 600036 10y's data.
</commit_message>
<xml_diff>
--- a/StockSmart/price.xlsx
+++ b/StockSmart/price.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <definedName name="_600036_6m" localSheetId="2">Sheet2!$A$55:$J$95</definedName>
     <definedName name="_600036_data1" localSheetId="2">Sheet2!$H$28:$Q$52</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="11">
   <si>
     <t>e</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -103,6 +103,10 @@
   </si>
   <si>
     <t>600036_36m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>60036_10year</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -155,14 +159,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1612,11 +1619,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="78419072"/>
-        <c:axId val="78421376"/>
+        <c:axId val="44881024"/>
+        <c:axId val="44883328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="78419072"/>
+        <c:axId val="44881024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1628,12 +1635,12 @@
         </c:title>
         <c:numFmt formatCode="0.0_ " sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78421376"/>
+        <c:crossAx val="44883328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="78421376"/>
+        <c:axId val="44883328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1648,7 +1655,7 @@
         <c:spPr>
           <a:ln w="6350"/>
         </c:spPr>
-        <c:crossAx val="78419072"/>
+        <c:crossAx val="44881024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1661,7 +1668,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1851,8 +1858,8 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="107332736"/>
-        <c:axId val="107334272"/>
+        <c:axId val="95450240"/>
+        <c:axId val="95451776"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -2032,11 +2039,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="107345792"/>
-        <c:axId val="107344256"/>
+        <c:axId val="95463296"/>
+        <c:axId val="95461760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="107332736"/>
+        <c:axId val="95450240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2044,12 +2051,12 @@
         <c:minorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107334272"/>
+        <c:crossAx val="95451776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="107334272"/>
+        <c:axId val="95451776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2086,12 +2093,12 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107332736"/>
+        <c:crossAx val="95450240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="107344256"/>
+        <c:axId val="95461760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2099,12 +2106,12 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107345792"/>
+        <c:crossAx val="95463296"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="107345792"/>
+        <c:axId val="95463296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2112,7 +2119,7 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="107344256"/>
+        <c:crossAx val="95461760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2125,7 +2132,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -2143,9 +2150,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="2.3288926141141263E-2"/>
-          <c:y val="2.9219145871408156E-2"/>
-          <c:w val="0.85960987220507368"/>
-          <c:h val="0.89543261539162267"/>
+          <c:y val="2.9219145871408159E-2"/>
+          <c:w val="0.85960987220507401"/>
+          <c:h val="0.89543261539162256"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2422,8 +2429,8 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="122802944"/>
-        <c:axId val="122804480"/>
+        <c:axId val="95511680"/>
+        <c:axId val="95513216"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -2699,11 +2706,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="122816000"/>
-        <c:axId val="122814464"/>
+        <c:axId val="95528832"/>
+        <c:axId val="95527296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="122802944"/>
+        <c:axId val="95511680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2711,12 +2718,12 @@
         <c:minorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122804480"/>
+        <c:crossAx val="95513216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="122804480"/>
+        <c:axId val="95513216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2753,12 +2760,12 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122802944"/>
+        <c:crossAx val="95511680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="122814464"/>
+        <c:axId val="95527296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2766,12 +2773,12 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122816000"/>
+        <c:crossAx val="95528832"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="122816000"/>
+        <c:axId val="95528832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2779,7 +2786,7 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="122814464"/>
+        <c:crossAx val="95527296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2792,10 +2799,2403 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="zh-CN"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="2.3288926141141263E-2"/>
+          <c:y val="2.9219145871408173E-2"/>
+          <c:w val="0.85960987220507468"/>
+          <c:h val="0.89543261539162256"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>count</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$C$1:$C$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-2.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-2.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1.9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-1.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1.7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-1.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-1.4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-1.3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-1.2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-0.9</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-0.8</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-0.7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-0.6</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-0.4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-0.3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-0.2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-0.1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$D$1:$D$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>249</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>594</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="120813824"/>
+        <c:axId val="120823808"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>avg</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$C:$C</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1048576"/>
+                <c:pt idx="0">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-2.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-2.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1.9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-1.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1.7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-1.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-1.4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-1.3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-1.2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-0.9</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-0.8</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-0.7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-0.6</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-0.4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-0.3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-0.2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-0.1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$G:$G</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1048576"/>
+                <c:pt idx="0">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.28</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.28</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.7370000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.56</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.8079999999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.333</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.857</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.3620000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.2530000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.2930000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.4239999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.1629999999999998</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.8540000000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.371</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.5680000000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.621</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.2559999999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.6020000000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.53</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.52</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.5409999999999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.357</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.498</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.4390000000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.8220000000000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.591</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.6870000000000001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.6379999999999999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.8779999999999999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.718</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.6830000000000001</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.581</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2.0099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2.1139999999999999</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.7390000000000001</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2.7210000000000001</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3.512</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.4670000000000001</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.7330000000000001</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2.44</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.6830000000000001</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3.2330000000000001</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.4750000000000001</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>6.05</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2.7330000000000001</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3.0329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="120826880"/>
+        <c:axId val="120825344"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="120813824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:minorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="120823808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="120823808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:tint val="66000"/>
+                      <a:satMod val="160000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:tint val="44500"/>
+                      <a:satMod val="160000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:tint val="23500"/>
+                      <a:satMod val="160000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="120813824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="120825344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="r"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="120826880"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="120826880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="none"/>
+        <c:crossAx val="120825344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="zh-CN"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>max</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>data!$F:$F</c:f>
+              <c:numCache>
+                <c:formatCode>0.0_ </c:formatCode>
+                <c:ptCount val="1048576"/>
+                <c:pt idx="0">
+                  <c:v>0.34310000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.8569</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.26319999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.6699999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2.226</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.62219999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.1600000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.27400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.36730000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.2100000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.90500000000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-9.0499999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.45500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-9.1700000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-0.182</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-0.27300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.1837</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.2399999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.36630000000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.36730000000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-0.183</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-2.2120000000000002</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-0.47299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-9.8500000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-9.8400000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-0.19819999999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.19670000000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>9.8299999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-9.9000000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-0.50049999999999994</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-0.51600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-0.20860000000000001</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.10440000000000001</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.31280000000000002</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.51280000000000003</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.40770000000000001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-0.1003</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>9.9900000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.2979</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.19839999999999999</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-0.29499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.19700000000000001</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-0.503</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-0.8982</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.1012</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.2039</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.1011</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-0.60360000000000003</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-0.1008</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-0.20280000000000001</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-9.9900000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-1.1976</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-0.19839999999999999</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>-0.41189999999999999</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.30830000000000002</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-0.29530000000000001</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>-0.19800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.2964</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>-9.8799999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.2964</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>-0.29620000000000002</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>-0.10009999999999999</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>-0.61160000000000003</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>-0.1013</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.51280000000000003</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>-0.69440000000000002</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>-9.8400000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1.0815999999999999</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>-0.19589999999999999</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.49020000000000002</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>9.6500000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>-0.19400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>9.7000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.67569999999999997</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>9.5299999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>-0.67049999999999998</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>-0.47849999999999998</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>-0.2868</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>-0.2918</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>9.8799999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>-0.1986</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>-0.19420000000000001</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>9.6000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>-0.58030000000000004</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>-9.8199999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0.39179999999999998</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>-0.29759999999999998</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>-0.1996</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0.3024</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>-0.30209999999999998</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0.40400000000000003</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>-0.4985</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>-0.20019999999999999</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>0.2006</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>-9.98E-2</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>0.20039999999999999</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>-9.6100000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>9.5699999999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>0.46300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>-0.18099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>0.55200000000000005</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>0.4274</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>-0.25619999999999998</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>-0.6734</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>0.16669999999999999</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>0.42020000000000002</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>-0.32629999999999998</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>-7.8299999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>0.46910000000000002</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>0.15859999999999999</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>0.5091</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>-0.22170000000000001</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>0.36759999999999998</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>-0.95660000000000001</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>-7.3899999999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>-0.82830000000000004</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>-0.28899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>-0.29010000000000002</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>7.3999999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>1.0589999999999999</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>0.374</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>-0.71430000000000005</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>0.5121</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>0.22270000000000001</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>7.0499999999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>6.8500000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>0.34770000000000001</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>-0.69930000000000003</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>-6.7699999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>-1.1668000000000001</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>-0.42430000000000001</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>0.64100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>-0.21510000000000001</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>0.21690000000000001</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>-1.3006</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>-0.22420000000000001</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>0.61209999999999998</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>-1.1503000000000001</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>0.39340000000000003</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>0.46729999999999999</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>-1.6832</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>0.48899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>7.4899999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>-0.5948</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>0.30509999999999998</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>-0.9002</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>-0.23680000000000001</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>7.8899999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>-0.71599999999999997</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>-0.2404</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>0.23810000000000001</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>0.45700000000000002</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>0.53310000000000002</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>-0.61629999999999996</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>-0.2364</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>-2.8974000000000002</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>0.49459999999999998</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>-1.1085</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>0.6452</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>0.31850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>-2.7364999999999999</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>0.63439999999999996</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>-7.9399999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>0.96460000000000001</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>0.16289999999999999</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>-0.40820000000000001</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>-0.16189999999999999</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>-0.90459999999999996</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>0.41120000000000001</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>-0.71319999999999995</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>0.47660000000000002</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>8.2400000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>-0.48780000000000001</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>0.49099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>-0.41149999999999998</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>0.49590000000000001</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>0.40489999999999998</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>-0.47889999999999999</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>-8.0100000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>0.56769999999999998</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>-7.8399999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>-7.5800000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>-7.4999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>-0.29430000000000001</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>-0.43290000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>data!$C:$C</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1048576"/>
+                <c:pt idx="0">
+                  <c:v>0.25640000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5748</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3853</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.54890000000000005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.92169999999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.55300000000000005</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.7599</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.72460000000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.72460000000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.4692000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.82040000000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.36499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.36659999999999998</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.5697000000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.2903</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.64039999999999997</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.36659999999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.2828</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.5917</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.8500000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.69579999999999997</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.5889</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.78510000000000002</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.99209999999999998</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.39560000000000001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9.9099999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.72609999999999997</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.83589999999999998</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.83420000000000005</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.4948000000000001</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.2244999999999999</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.2182999999999999</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.80649999999999999</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.1044</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.3992</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.39960000000000001</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.79920000000000002</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.99009999999999998</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.5917</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.68830000000000002</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.19670000000000001</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.80889999999999995</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.3105</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.90629999999999999</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.50560000000000005</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.71209999999999996</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.70709999999999995</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.1133999999999999</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.30270000000000002</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2.3374000000000001</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2.5253000000000001</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.59230000000000005</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.59640000000000004</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>9.9900000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.72389999999999999</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>4.3033000000000001</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.59230000000000005</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.39679999999999999</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.68969999999999998</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.89019999999999999</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1.7734000000000001</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>9.7600000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.1002</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.30399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1.3347</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1.641</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.30430000000000001</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.5071</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>3.8776000000000002</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1.6982999999999999</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1.9703999999999999</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.87549999999999994</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.49070000000000003</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1.3658999999999999</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>9.64E-2</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.87460000000000004</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.7752</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>1.0547</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1.7358</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.85629999999999995</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.86539999999999995</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.57530000000000003</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.5786</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.1951</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>1.0859000000000001</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.59699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>3.1745999999999999</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>1.07</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>1.1572</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.38350000000000001</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.3891</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.78659999999999997</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0.39019999999999999</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>9.7500000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0.497</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0.39800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>0.20080000000000001</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0.70350000000000001</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>1.119</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>0.30299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>1.1066</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>0.40079999999999999</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>0.8024</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>0.50149999999999995</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>0.50049999999999994</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>0.70140000000000002</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>9.9900000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>1.0091000000000001</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>1.5385</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>3.5373000000000001</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>2.1198000000000001</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>0.82040000000000002</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>2.0017999999999998</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>0.27200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>7.5023</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>1.617</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>3.4247000000000001</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>1.6878</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>2.3729</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>0.33279999999999998</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>3.8494000000000002</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>5.9737999999999998</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>1.4107000000000001</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>1.323</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>2.7711999999999999</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>6.4814999999999996</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>1.0853999999999999</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>2.4443999999999999</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>1.3187</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>1.1887000000000001</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>1.4815</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>0.81299999999999994</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>6.0743999999999998</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>0.57969999999999999</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>0.5091</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>7.3899999999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>1.0479000000000001</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>2.0863999999999998</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>3.8319999999999999</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>1.5107999999999999</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>3.5714000000000001</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>0.65500000000000003</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>6.2222</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>4.2988</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>0.20530000000000001</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>0.4158</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>4.5069999999999997</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>1.6249</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>0.97219999999999995</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>0.83330000000000004</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>0.71020000000000005</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>0.99080000000000001</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>1.0057</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>0.36080000000000001</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>0.1464</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>0.22470000000000001</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>0.83650000000000002</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>3.0255999999999998</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>1.8809</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>3.2557999999999998</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>0.52629999999999999</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>1.1673</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>9.2456999999999994</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>1.7202999999999999</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>2.5095000000000001</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>0.15140000000000001</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>1.3720000000000001</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>1.0078</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>1.8987000000000001</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>4.0221</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>1.7627999999999999</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>1.7670999999999999</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>4.2755000000000001</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>0.60880000000000001</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>0.45490000000000003</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>0.60609999999999997</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>0.3876</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>2.0537000000000001</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>4.5118999999999998</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>0.96079999999999999</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>2.1635</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>3.0158999999999998</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>2.0095999999999998</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>0.70920000000000005</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>0.55640000000000001</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>0.63690000000000002</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>0.56499999999999995</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>0.81299999999999994</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>1.6393</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>0.16220000000000001</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>2.0747</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>5.1597</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>0.87790000000000001</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>2.4691000000000001</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>0.89870000000000005</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>0.48859999999999998</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>0.1653</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>3.2071999999999998</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>2.0160999999999998</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>0.48120000000000002</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>1.3622000000000001</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>0.31900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>3.0644999999999998</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>3.6892</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>1.3656999999999999</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>2.4775</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>2.8782000000000001</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>0.43259999999999998</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>1.7316</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>7.2499999999999995E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="111268608"/>
+        <c:axId val="111271296"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="111268608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="0.0_ " sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="111271296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="111271296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6350"/>
+        </c:spPr>
+        <c:crossAx val="111268608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -2891,6 +5291,66 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="图表 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>163</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2924,10 +5384,10 @@
         <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
-            <a:t>60036 6m high</a:t>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="1"/>
+            <a:t>600036 6m high</a:t>
           </a:r>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100" b="1"/>
         </a:p>
       </cdr:txBody>
     </cdr:sp>
@@ -2965,10 +5425,54 @@
         <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
-            <a:t>60036 36m high</a:t>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="1"/>
+            <a:t>600036 36m high</a:t>
           </a:r>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.07881</cdr:x>
+      <cdr:y>0.1128</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.26407</cdr:x>
+      <cdr:y>0.21692</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="733425" y="495308"/>
+          <a:ext cx="1723991" cy="457193"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1"/>
+            <a:t>600036 10y high</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1"/>
         </a:p>
       </cdr:txBody>
     </cdr:sp>
@@ -2989,7 +5493,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -7286,8 +9790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="F22"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="P72" sqref="P72"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="B129" sqref="B129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -7308,7 +9812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A28:Q95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
@@ -9457,12 +11961,1038 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4">
+        <v>-3</v>
+      </c>
+      <c r="D1" s="4">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="F1" s="4">
+        <v>0</v>
+      </c>
+      <c r="G1" s="4">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="C2" s="4">
+        <v>-2.9</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="C3" s="4">
+        <v>-2.8</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F3" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G3" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="C4" s="4">
+        <v>-2.7</v>
+      </c>
+      <c r="D4" s="4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2.7</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="G4" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="C5" s="4">
+        <v>-2.6</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3</v>
+      </c>
+      <c r="E5" s="4">
+        <v>6.4</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="G5" s="4">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="C6" s="4">
+        <v>-2.5</v>
+      </c>
+      <c r="D6" s="4">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4">
+        <v>7.1</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="G6" s="4">
+        <v>4.28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="C7" s="4">
+        <v>-2.4</v>
+      </c>
+      <c r="D7" s="4">
+        <v>5</v>
+      </c>
+      <c r="E7" s="4">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="G7" s="4">
+        <v>4.28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="C8" s="4">
+        <v>-2.2999999999999998</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2</v>
+      </c>
+      <c r="E8" s="4">
+        <v>5.7</v>
+      </c>
+      <c r="F8" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G8" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="C9" s="4">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="D9" s="4">
+        <v>8</v>
+      </c>
+      <c r="E9" s="4">
+        <v>11.3</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>3.7370000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="C10" s="4">
+        <v>-2.1</v>
+      </c>
+      <c r="D10" s="4">
+        <v>5</v>
+      </c>
+      <c r="E10" s="4">
+        <v>4.3</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1.56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="C11" s="4">
+        <v>-2</v>
+      </c>
+      <c r="D11" s="4">
+        <v>12</v>
+      </c>
+      <c r="E11" s="4">
+        <v>10.6</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+      <c r="G11" s="4">
+        <v>2.8079999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="C12" s="4">
+        <v>-1.9</v>
+      </c>
+      <c r="D12" s="4">
+        <v>6</v>
+      </c>
+      <c r="E12" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1.333</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="C13" s="4">
+        <v>-1.8</v>
+      </c>
+      <c r="D13" s="4">
+        <v>7</v>
+      </c>
+      <c r="E13" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="G13" s="4">
+        <v>1.857</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="C14" s="4">
+        <v>-1.7</v>
+      </c>
+      <c r="D14" s="4">
+        <v>13</v>
+      </c>
+      <c r="E14" s="4">
+        <v>5</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14" s="4">
+        <v>2.3620000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="C15" s="4">
+        <v>-1.6</v>
+      </c>
+      <c r="D15" s="4">
+        <v>11</v>
+      </c>
+      <c r="E15" s="4">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="C16" s="4">
+        <v>-1.5</v>
+      </c>
+      <c r="D16" s="4">
+        <v>15</v>
+      </c>
+      <c r="E16" s="4">
+        <v>5.7</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
+        <v>2.2530000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7">
+      <c r="C17" s="4">
+        <v>-1.4</v>
+      </c>
+      <c r="D17" s="4">
+        <v>15</v>
+      </c>
+      <c r="E17" s="4">
+        <v>5.9</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G17" s="4">
+        <v>2.2930000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7">
+      <c r="C18" s="4">
+        <v>-1.3</v>
+      </c>
+      <c r="D18" s="4">
+        <v>25</v>
+      </c>
+      <c r="E18" s="4">
+        <v>4.3</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0</v>
+      </c>
+      <c r="G18" s="4">
+        <v>1.4239999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7">
+      <c r="C19" s="4">
+        <v>-1.2</v>
+      </c>
+      <c r="D19" s="4">
+        <v>16</v>
+      </c>
+      <c r="E19" s="4">
+        <v>5.2</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0</v>
+      </c>
+      <c r="G19" s="4">
+        <v>2.1629999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7">
+      <c r="C20" s="4">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="D20" s="4">
+        <v>28</v>
+      </c>
+      <c r="E20" s="4">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0</v>
+      </c>
+      <c r="G20" s="4">
+        <v>2.8540000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7">
+      <c r="C21" s="4">
+        <v>-1</v>
+      </c>
+      <c r="D21" s="4">
+        <v>17</v>
+      </c>
+      <c r="E21" s="4">
+        <v>7.4</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G21" s="4">
+        <v>2.371</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7">
+      <c r="C22" s="4">
+        <v>-0.9</v>
+      </c>
+      <c r="D22" s="4">
+        <v>38</v>
+      </c>
+      <c r="E22" s="4">
+        <v>5.3</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0</v>
+      </c>
+      <c r="G22" s="4">
+        <v>1.5680000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7">
+      <c r="C23" s="4">
+        <v>-0.8</v>
+      </c>
+      <c r="D23" s="4">
+        <v>53</v>
+      </c>
+      <c r="E23" s="4">
+        <v>6.1</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0</v>
+      </c>
+      <c r="G23" s="4">
+        <v>1.621</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7">
+      <c r="C24" s="4">
+        <v>-0.7</v>
+      </c>
+      <c r="D24" s="4">
+        <v>57</v>
+      </c>
+      <c r="E24" s="4">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="F24" s="4">
+        <v>0</v>
+      </c>
+      <c r="G24" s="4">
+        <v>2.2559999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7">
+      <c r="C25" s="4">
+        <v>-0.6</v>
+      </c>
+      <c r="D25" s="4">
+        <v>47</v>
+      </c>
+      <c r="E25" s="4">
+        <v>6.3</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0</v>
+      </c>
+      <c r="G25" s="4">
+        <v>1.6020000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7">
+      <c r="C26" s="4">
+        <v>-0.5</v>
+      </c>
+      <c r="D26" s="4">
+        <v>70</v>
+      </c>
+      <c r="E26" s="4">
+        <v>6.1</v>
+      </c>
+      <c r="F26" s="4">
+        <v>0</v>
+      </c>
+      <c r="G26" s="4">
+        <v>1.53</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7">
+      <c r="C27" s="4">
+        <v>-0.4</v>
+      </c>
+      <c r="D27" s="4">
+        <v>96</v>
+      </c>
+      <c r="E27" s="4">
+        <v>5.7</v>
+      </c>
+      <c r="F27" s="4">
+        <v>0</v>
+      </c>
+      <c r="G27" s="4">
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7">
+      <c r="C28" s="4">
+        <v>-0.3</v>
+      </c>
+      <c r="D28" s="4">
+        <v>91</v>
+      </c>
+      <c r="E28" s="4">
+        <v>10.3</v>
+      </c>
+      <c r="F28" s="4">
+        <v>0</v>
+      </c>
+      <c r="G28" s="4">
+        <v>1.5409999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="3:7">
+      <c r="C29" s="4">
+        <v>-0.2</v>
+      </c>
+      <c r="D29" s="4">
+        <v>249</v>
+      </c>
+      <c r="E29" s="4">
+        <v>8</v>
+      </c>
+      <c r="F29" s="4">
+        <v>0</v>
+      </c>
+      <c r="G29" s="4">
+        <v>1.357</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7">
+      <c r="C30" s="4">
+        <v>-0.1</v>
+      </c>
+      <c r="D30" s="4">
+        <v>112</v>
+      </c>
+      <c r="E30" s="4">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="F30" s="4">
+        <v>0</v>
+      </c>
+      <c r="G30" s="4">
+        <v>1.498</v>
+      </c>
+    </row>
+    <row r="31" spans="3:7">
+      <c r="C31" s="4">
+        <v>0</v>
+      </c>
+      <c r="D31" s="4">
+        <v>594</v>
+      </c>
+      <c r="E31" s="4">
+        <v>10</v>
+      </c>
+      <c r="F31" s="4">
+        <v>0</v>
+      </c>
+      <c r="G31" s="4">
+        <v>1.4390000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7">
+      <c r="C32" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D32" s="4">
+        <v>122</v>
+      </c>
+      <c r="E32" s="4">
+        <v>8</v>
+      </c>
+      <c r="F32" s="4">
+        <v>0</v>
+      </c>
+      <c r="G32" s="4">
+        <v>1.8220000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7">
+      <c r="C33" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="D33" s="4">
+        <v>232</v>
+      </c>
+      <c r="E33" s="4">
+        <v>9.4</v>
+      </c>
+      <c r="F33" s="4">
+        <v>0</v>
+      </c>
+      <c r="G33" s="4">
+        <v>1.591</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7">
+      <c r="C34" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="D34" s="4">
+        <v>105</v>
+      </c>
+      <c r="E34" s="4">
+        <v>7</v>
+      </c>
+      <c r="F34" s="4">
+        <v>0</v>
+      </c>
+      <c r="G34" s="4">
+        <v>1.6870000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7">
+      <c r="C35" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="D35" s="4">
+        <v>92</v>
+      </c>
+      <c r="E35" s="4">
+        <v>5.9</v>
+      </c>
+      <c r="F35" s="4">
+        <v>0</v>
+      </c>
+      <c r="G35" s="4">
+        <v>1.6379999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7">
+      <c r="C36" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D36" s="4">
+        <v>82</v>
+      </c>
+      <c r="E36" s="4">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="F36" s="4">
+        <v>0</v>
+      </c>
+      <c r="G36" s="4">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7">
+      <c r="C37" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="D37" s="4">
+        <v>69</v>
+      </c>
+      <c r="E37" s="4">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="F37" s="4">
+        <v>0</v>
+      </c>
+      <c r="G37" s="4">
+        <v>1.8779999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7">
+      <c r="C38" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="D38" s="4">
+        <v>50</v>
+      </c>
+      <c r="E38" s="4">
+        <v>6</v>
+      </c>
+      <c r="F38" s="4">
+        <v>0</v>
+      </c>
+      <c r="G38" s="4">
+        <v>1.718</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7">
+      <c r="C39" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="D39" s="4">
+        <v>35</v>
+      </c>
+      <c r="E39" s="4">
+        <v>4.3</v>
+      </c>
+      <c r="F39" s="4">
+        <v>0</v>
+      </c>
+      <c r="G39" s="4">
+        <v>1.6830000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7">
+      <c r="C40" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="D40" s="4">
+        <v>31</v>
+      </c>
+      <c r="E40" s="4">
+        <v>5.4</v>
+      </c>
+      <c r="F40" s="4">
+        <v>0</v>
+      </c>
+      <c r="G40" s="4">
+        <v>1.581</v>
+      </c>
+    </row>
+    <row r="41" spans="3:7">
+      <c r="C41" s="4">
+        <v>1</v>
+      </c>
+      <c r="D41" s="4">
+        <v>21</v>
+      </c>
+      <c r="E41" s="4">
+        <v>6.5</v>
+      </c>
+      <c r="F41" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="G41" s="4">
+        <v>2.0099999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="3:7">
+      <c r="C42" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D42" s="4">
+        <v>20</v>
+      </c>
+      <c r="E42" s="4">
+        <v>6.9</v>
+      </c>
+      <c r="F42" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G42" s="4">
+        <v>2.02</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7">
+      <c r="C43" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="D43" s="4">
+        <v>14</v>
+      </c>
+      <c r="E43" s="4">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="F43" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="G43" s="4">
+        <v>2.1139999999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="3:7">
+      <c r="C44" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="D44" s="4">
+        <v>18</v>
+      </c>
+      <c r="E44" s="4">
+        <v>5.5</v>
+      </c>
+      <c r="F44" s="4">
+        <v>0</v>
+      </c>
+      <c r="G44" s="4">
+        <v>1.7390000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="3:7">
+      <c r="C45" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="D45" s="4">
+        <v>14</v>
+      </c>
+      <c r="E45" s="4">
+        <v>8.4</v>
+      </c>
+      <c r="F45" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="G45" s="4">
+        <v>2.7210000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="3:7">
+      <c r="C46" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="D46" s="4">
+        <v>8</v>
+      </c>
+      <c r="E46" s="4">
+        <v>8.5</v>
+      </c>
+      <c r="F46" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G46" s="4">
+        <v>3.512</v>
+      </c>
+    </row>
+    <row r="47" spans="3:7">
+      <c r="C47" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="D47" s="4">
+        <v>5</v>
+      </c>
+      <c r="E47" s="4">
+        <v>6.8</v>
+      </c>
+      <c r="F47" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="G47" s="4">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="48" spans="3:7">
+      <c r="C48" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="D48" s="4">
+        <v>3</v>
+      </c>
+      <c r="E48" s="4">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F48" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="G48" s="4">
+        <v>2.4670000000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="3:7">
+      <c r="C49" s="4">
+        <v>1.8</v>
+      </c>
+      <c r="D49" s="4">
+        <v>6</v>
+      </c>
+      <c r="E49" s="4">
+        <v>6.6</v>
+      </c>
+      <c r="F49" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="G49" s="4">
+        <v>1.7330000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="3:7">
+      <c r="C50" s="4">
+        <v>1.9</v>
+      </c>
+      <c r="D50" s="4">
+        <v>8</v>
+      </c>
+      <c r="E50" s="4">
+        <v>5.4</v>
+      </c>
+      <c r="F50" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="G50" s="4">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="51" spans="3:7">
+      <c r="C51" s="4">
+        <v>2</v>
+      </c>
+      <c r="D51" s="4">
+        <v>5</v>
+      </c>
+      <c r="E51" s="4">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F51" s="4">
+        <v>0</v>
+      </c>
+      <c r="G51" s="4">
+        <v>2.44</v>
+      </c>
+    </row>
+    <row r="52" spans="3:7">
+      <c r="C52" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="D52" s="4">
+        <v>6</v>
+      </c>
+      <c r="E52" s="4">
+        <v>4.7</v>
+      </c>
+      <c r="F52" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G52" s="4">
+        <v>1.6830000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="3:7">
+      <c r="C53" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D53" s="4">
+        <v>3</v>
+      </c>
+      <c r="E53" s="4">
+        <v>5.4</v>
+      </c>
+      <c r="F53" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="G53" s="4">
+        <v>3.2330000000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="3:7">
+      <c r="C54" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D54" s="4">
+        <v>4</v>
+      </c>
+      <c r="E54" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="F54" s="4">
+        <v>0</v>
+      </c>
+      <c r="G54" s="4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="55" spans="3:7">
+      <c r="C55" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="D55" s="4">
+        <v>4</v>
+      </c>
+      <c r="E55" s="4">
+        <v>2.9</v>
+      </c>
+      <c r="F55" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G55" s="4">
+        <v>1.4750000000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="3:7">
+      <c r="C56" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="D56" s="4">
+        <v>2</v>
+      </c>
+      <c r="E56" s="4">
+        <v>7.3</v>
+      </c>
+      <c r="F56" s="4">
+        <v>4.8</v>
+      </c>
+      <c r="G56" s="4">
+        <v>6.05</v>
+      </c>
+    </row>
+    <row r="57" spans="3:7">
+      <c r="C57" s="4">
+        <v>2.6</v>
+      </c>
+      <c r="D57" s="4">
+        <v>3</v>
+      </c>
+      <c r="E57" s="4">
+        <v>7.2</v>
+      </c>
+      <c r="F57" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="G57" s="4">
+        <v>2.7330000000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="3:7">
+      <c r="C58" s="4">
+        <v>2.7</v>
+      </c>
+      <c r="D58" s="4">
+        <v>1</v>
+      </c>
+      <c r="E58" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="F58" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="G58" s="4">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="59" spans="3:7">
+      <c r="C59" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="D59" s="4">
+        <v>3</v>
+      </c>
+      <c r="E59" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="F59" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="G59" s="4">
+        <v>3.0329999999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="3:7">
+      <c r="C60" s="4">
+        <v>2.9</v>
+      </c>
+      <c r="D60" s="4">
+        <v>1</v>
+      </c>
+      <c r="E60" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F60" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G60" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
get listHigh and listLow.
</commit_message>
<xml_diff>
--- a/StockSmart/price.xlsx
+++ b/StockSmart/price.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -17,7 +17,7 @@
     <definedName name="_600036_6m" localSheetId="2">Sheet2!$A$55:$J$95</definedName>
     <definedName name="_600036_data1" localSheetId="2">Sheet2!$H$28:$Q$52</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -169,7 +169,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1619,11 +1619,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="44881024"/>
-        <c:axId val="44883328"/>
+        <c:axId val="70620288"/>
+        <c:axId val="70622592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44881024"/>
+        <c:axId val="70620288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1635,12 +1635,12 @@
         </c:title>
         <c:numFmt formatCode="0.0_ " sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44883328"/>
+        <c:crossAx val="70622592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44883328"/>
+        <c:axId val="70622592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1655,7 +1655,7 @@
         <c:spPr>
           <a:ln w="6350"/>
         </c:spPr>
-        <c:crossAx val="44881024"/>
+        <c:crossAx val="70620288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1668,7 +1668,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1858,8 +1858,8 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="95450240"/>
-        <c:axId val="95451776"/>
+        <c:axId val="98800768"/>
+        <c:axId val="98802304"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -2039,11 +2039,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="95463296"/>
-        <c:axId val="95461760"/>
+        <c:axId val="98817920"/>
+        <c:axId val="98816384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95450240"/>
+        <c:axId val="98800768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2051,12 +2051,12 @@
         <c:minorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95451776"/>
+        <c:crossAx val="98802304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95451776"/>
+        <c:axId val="98802304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2093,12 +2093,12 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95450240"/>
+        <c:crossAx val="98800768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95461760"/>
+        <c:axId val="98816384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2106,12 +2106,12 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95463296"/>
+        <c:crossAx val="98817920"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95463296"/>
+        <c:axId val="98817920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2119,7 +2119,7 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="95461760"/>
+        <c:crossAx val="98816384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2132,7 +2132,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -2150,8 +2150,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="2.3288926141141263E-2"/>
-          <c:y val="2.9219145871408159E-2"/>
-          <c:w val="0.85960987220507401"/>
+          <c:y val="2.9219145871408163E-2"/>
+          <c:w val="0.85960987220507434"/>
           <c:h val="0.89543261539162256"/>
         </c:manualLayout>
       </c:layout>
@@ -2429,8 +2429,8 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="95511680"/>
-        <c:axId val="95513216"/>
+        <c:axId val="98878592"/>
+        <c:axId val="98880128"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -2706,11 +2706,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="95528832"/>
-        <c:axId val="95527296"/>
+        <c:axId val="98895744"/>
+        <c:axId val="98894208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95511680"/>
+        <c:axId val="98878592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2718,12 +2718,12 @@
         <c:minorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95513216"/>
+        <c:crossAx val="98880128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95513216"/>
+        <c:axId val="98880128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2760,12 +2760,12 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95511680"/>
+        <c:crossAx val="98878592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95527296"/>
+        <c:axId val="98894208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2773,12 +2773,12 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95528832"/>
+        <c:crossAx val="98895744"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95528832"/>
+        <c:axId val="98895744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2786,7 +2786,7 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="95527296"/>
+        <c:crossAx val="98894208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2799,7 +2799,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -2817,8 +2817,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="2.3288926141141263E-2"/>
-          <c:y val="2.9219145871408173E-2"/>
-          <c:w val="0.85960987220507468"/>
+          <c:y val="2.921914587140818E-2"/>
+          <c:w val="0.85960987220507501"/>
           <c:h val="0.89543261539162256"/>
         </c:manualLayout>
       </c:layout>
@@ -3210,8 +3210,8 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="120813824"/>
-        <c:axId val="120823808"/>
+        <c:axId val="98941952"/>
+        <c:axId val="98943744"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -3219,7 +3219,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>avg</c:v>
+            <c:v>avgH</c:v>
           </c:tx>
           <c:xVal>
             <c:numRef>
@@ -3601,11 +3601,397 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="120826880"/>
-        <c:axId val="120825344"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>avgL</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$C:$C</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1048576"/>
+                <c:pt idx="0">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-2.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-2.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1.9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-1.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1.7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-1.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-1.4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-1.3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-1.2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-0.9</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-0.8</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-0.7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-0.6</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-0.4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-0.3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-0.2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-0.1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$K:$K</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1048576"/>
+                <c:pt idx="0">
+                  <c:v>-2.9329999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-5.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2.367</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1.44</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.98</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.85</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1.5629999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-4.12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-2.2669999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-2.4500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-1.871</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1.6619999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1.6910000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-1.653</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-2.2069999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-1.419</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-1.464</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-1.7529999999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-1.911</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-1.3420000000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-1.4159999999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-1.5740000000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-1.679</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-1.306</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-1.3560000000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-1.343</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-1.5760000000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-1.286</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-1.2869999999999999</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-1.238</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-1.163</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-1.236</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-1.3959999999999999</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-1.8480000000000001</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-1.6359999999999999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-1.6140000000000001</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-1.8</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-1.69</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-1.47</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-2.1859999999999999</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-1.744</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-1.8069999999999999</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-1.2130000000000001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-1.2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-4.1669999999999998</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-1.9830000000000001</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-2.2629999999999999</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-2.72</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-1.833</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-0.9</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-2.4750000000000001</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-4.4749999999999996</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-0.7</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-2.8</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-3.2</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-2.9670000000000001</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-3.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="98955264"/>
+        <c:axId val="98945280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="120813824"/>
+        <c:axId val="98941952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3613,12 +3999,12 @@
         <c:minorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120823808"/>
+        <c:crossAx val="98943744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="120823808"/>
+        <c:axId val="98943744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3655,12 +4041,12 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120813824"/>
+        <c:crossAx val="98941952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="120825344"/>
+        <c:axId val="98945280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3668,12 +4054,12 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120826880"/>
+        <c:crossAx val="98955264"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="120826880"/>
+        <c:axId val="98955264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3681,7 +4067,7 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="120825344"/>
+        <c:crossAx val="98945280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3694,1508 +4080,10 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="zh-CN"/>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>max</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:xVal>
-            <c:numRef>
-              <c:f>data!$F:$F</c:f>
-              <c:numCache>
-                <c:formatCode>0.0_ </c:formatCode>
-                <c:ptCount val="1048576"/>
-                <c:pt idx="0">
-                  <c:v>0.34310000000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-0.8569</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.26319999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.6699999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-2.226</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-0.62219999999999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9.1600000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-0.27400000000000002</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.37</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-0.36730000000000002</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>9.2100000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.90500000000000003</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-9.0499999999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.45500000000000002</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-9.1700000000000004E-2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-0.182</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-0.27300000000000002</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.1837</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>9.2399999999999996E-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.36630000000000001</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.36730000000000002</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>-0.183</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>-2.2120000000000002</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>-0.47299999999999998</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>-9.8500000000000004E-2</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>-9.8400000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>-0.19819999999999999</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.19670000000000001</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>9.8299999999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>-9.9000000000000005E-2</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>-0.50049999999999994</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>-0.51600000000000001</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>-0.20860000000000001</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.10440000000000001</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.31280000000000002</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.51280000000000003</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.40770000000000001</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>-0.1003</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>9.9900000000000003E-2</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.2979</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.19839999999999999</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>-0.29499999999999998</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>0.19700000000000001</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>-0.503</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>-0.8982</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>0.1012</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0.2039</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>0.1011</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>-0.60360000000000003</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>-0.1008</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>-0.20280000000000001</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>-9.9900000000000003E-2</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>-1.1976</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>-0.19839999999999999</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>-0.41189999999999999</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>0.30830000000000002</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>-0.29530000000000001</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>-0.19800000000000001</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>0.2964</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>-9.8799999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>0.2964</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>-0.29620000000000002</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>-0.10009999999999999</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>-0.61160000000000003</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>-0.1013</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>0.51280000000000003</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>-0.69440000000000002</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>-9.8400000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>1.0815999999999999</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>-0.19589999999999999</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>0.49020000000000002</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>9.6500000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>-0.19400000000000001</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>9.7000000000000003E-2</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>0.67569999999999997</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>9.5299999999999996E-2</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>-0.67049999999999998</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>-0.47849999999999998</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>-0.2868</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>-0.2918</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>9.8799999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>-0.1986</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>-0.19420000000000001</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>9.6000000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>-0.58030000000000004</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>-9.8199999999999996E-2</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>0.39179999999999998</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>-0.29759999999999998</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>-0.1996</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>0.3024</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>-0.30209999999999998</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>0.40400000000000003</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>-0.4985</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>-0.20019999999999999</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>0.2006</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>-9.98E-2</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>0.20039999999999999</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>-9.6100000000000005E-2</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>9.5699999999999993E-2</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>0.46300000000000002</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>-0.18099999999999999</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>0.55200000000000005</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>0.4274</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>-0.25619999999999998</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>-0.6734</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>0.16669999999999999</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>0.42020000000000002</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>-0.32629999999999998</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>-7.8299999999999995E-2</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>0.46910000000000002</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>0.15859999999999999</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>0.5091</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>-0.22170000000000001</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>0.36759999999999998</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>-0.95660000000000001</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>-7.3899999999999993E-2</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>-0.82830000000000004</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>-0.28899999999999998</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>-0.29010000000000002</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>7.3999999999999996E-2</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>1.0589999999999999</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>0.374</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>-0.71430000000000005</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>0.5121</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>0.22270000000000001</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>7.0499999999999993E-2</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>6.8500000000000005E-2</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>0.34770000000000001</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>-0.69930000000000003</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>-6.7699999999999996E-2</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>-1.1668000000000001</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>-0.42430000000000001</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>0.64100000000000001</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>-0.21510000000000001</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>0.21690000000000001</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>-1.3006</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>-0.22420000000000001</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>0.61209999999999998</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>-1.1503000000000001</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>0.39340000000000003</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>0.46729999999999999</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>-1.6832</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>0.48899999999999999</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>7.4899999999999994E-2</c:v>
-                </c:pt>
-                <c:pt idx="185">
-                  <c:v>-0.5948</c:v>
-                </c:pt>
-                <c:pt idx="186">
-                  <c:v>0.30509999999999998</c:v>
-                </c:pt>
-                <c:pt idx="187">
-                  <c:v>-0.9002</c:v>
-                </c:pt>
-                <c:pt idx="188">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="189">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="190">
-                  <c:v>-0.23680000000000001</c:v>
-                </c:pt>
-                <c:pt idx="191">
-                  <c:v>7.8899999999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="192">
-                  <c:v>-0.71599999999999997</c:v>
-                </c:pt>
-                <c:pt idx="193">
-                  <c:v>-0.2404</c:v>
-                </c:pt>
-                <c:pt idx="194">
-                  <c:v>0.23810000000000001</c:v>
-                </c:pt>
-                <c:pt idx="195">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="196">
-                  <c:v>0.45700000000000002</c:v>
-                </c:pt>
-                <c:pt idx="197">
-                  <c:v>0.53310000000000002</c:v>
-                </c:pt>
-                <c:pt idx="198">
-                  <c:v>-0.61629999999999996</c:v>
-                </c:pt>
-                <c:pt idx="199">
-                  <c:v>-0.2364</c:v>
-                </c:pt>
-                <c:pt idx="200">
-                  <c:v>-2.8974000000000002</c:v>
-                </c:pt>
-                <c:pt idx="201">
-                  <c:v>0.49459999999999998</c:v>
-                </c:pt>
-                <c:pt idx="202">
-                  <c:v>-1.1085</c:v>
-                </c:pt>
-                <c:pt idx="203">
-                  <c:v>0.6452</c:v>
-                </c:pt>
-                <c:pt idx="204">
-                  <c:v>0.31850000000000001</c:v>
-                </c:pt>
-                <c:pt idx="205">
-                  <c:v>-2.7364999999999999</c:v>
-                </c:pt>
-                <c:pt idx="206">
-                  <c:v>0.63439999999999996</c:v>
-                </c:pt>
-                <c:pt idx="207">
-                  <c:v>-7.9399999999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="208">
-                  <c:v>0.96460000000000001</c:v>
-                </c:pt>
-                <c:pt idx="209">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="210">
-                  <c:v>0.16289999999999999</c:v>
-                </c:pt>
-                <c:pt idx="211">
-                  <c:v>-0.40820000000000001</c:v>
-                </c:pt>
-                <c:pt idx="212">
-                  <c:v>-0.16189999999999999</c:v>
-                </c:pt>
-                <c:pt idx="213">
-                  <c:v>-0.90459999999999996</c:v>
-                </c:pt>
-                <c:pt idx="214">
-                  <c:v>0.41120000000000001</c:v>
-                </c:pt>
-                <c:pt idx="215">
-                  <c:v>-0.71319999999999995</c:v>
-                </c:pt>
-                <c:pt idx="216">
-                  <c:v>0.47660000000000002</c:v>
-                </c:pt>
-                <c:pt idx="217">
-                  <c:v>8.2400000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="218">
-                  <c:v>-0.48780000000000001</c:v>
-                </c:pt>
-                <c:pt idx="219">
-                  <c:v>0.49099999999999999</c:v>
-                </c:pt>
-                <c:pt idx="220">
-                  <c:v>-0.41149999999999998</c:v>
-                </c:pt>
-                <c:pt idx="221">
-                  <c:v>0.49590000000000001</c:v>
-                </c:pt>
-                <c:pt idx="222">
-                  <c:v>0.40489999999999998</c:v>
-                </c:pt>
-                <c:pt idx="223">
-                  <c:v>-0.47889999999999999</c:v>
-                </c:pt>
-                <c:pt idx="224">
-                  <c:v>-8.0100000000000005E-2</c:v>
-                </c:pt>
-                <c:pt idx="225">
-                  <c:v>0.32</c:v>
-                </c:pt>
-                <c:pt idx="226">
-                  <c:v>0.56769999999999998</c:v>
-                </c:pt>
-                <c:pt idx="227">
-                  <c:v>-7.8399999999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="228">
-                  <c:v>-7.5800000000000006E-2</c:v>
-                </c:pt>
-                <c:pt idx="229">
-                  <c:v>-7.4999999999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="230">
-                  <c:v>-0.29430000000000001</c:v>
-                </c:pt>
-                <c:pt idx="231">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="232">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="233">
-                  <c:v>-0.43290000000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>data!$C:$C</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1048576"/>
-                <c:pt idx="0">
-                  <c:v>0.25640000000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.5748</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.3853</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.54890000000000005</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.92169999999999996</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.55300000000000005</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2.7599</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.72460000000000002</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.72460000000000002</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.4692000000000001</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.82040000000000002</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.36499999999999999</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.36659999999999998</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1.5697000000000001</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1.2903</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.64039999999999997</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.36659999999999998</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.2828</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.5917</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>9.8500000000000004E-2</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.69579999999999997</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1.5889</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.78510000000000002</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.99209999999999998</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.39560000000000001</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>9.9099999999999994E-2</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.72609999999999997</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.83589999999999998</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.83420000000000005</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>2.4948000000000001</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>1.2244999999999999</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>1.2182999999999999</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.80649999999999999</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>1.1044</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.3992</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.39960000000000001</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0.79920000000000002</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.99009999999999998</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.5917</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>0.68830000000000002</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>0.19670000000000001</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>0.80889999999999995</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>1.3105</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>0.90629999999999999</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>0.50560000000000005</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0.71209999999999996</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>0.70709999999999995</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>1.1133999999999999</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>0.30270000000000002</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>2.3374000000000001</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>2.5253000000000001</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>0.59230000000000005</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>0.59640000000000004</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>9.9900000000000003E-2</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>0.72389999999999999</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>4.3033000000000001</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>0.59230000000000005</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>0.39679999999999999</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>0.68969999999999998</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>0.89019999999999999</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>1.7734000000000001</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>9.7600000000000006E-2</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>0.1002</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>0.30399999999999999</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>1.3347</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>1.641</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>0.30430000000000001</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>0.5071</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>3.8776000000000002</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>1.6982999999999999</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>1.9703999999999999</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>0.87549999999999994</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>0.49070000000000003</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>1.3658999999999999</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>9.64E-2</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>0.87460000000000004</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>0.7752</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>1.0547</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>1.7358</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>0.85629999999999995</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>0.86539999999999995</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>0.57530000000000003</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>0.5786</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>0.1951</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>1.0859000000000001</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>0.59699999999999998</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>3.1745999999999999</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>1.07</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>1.1572</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>0.38350000000000001</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>0.3891</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>0.78659999999999997</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>0.39019999999999999</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>9.7500000000000003E-2</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>0.497</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>0.39800000000000002</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>0.20080000000000001</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>0.70350000000000001</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>1.119</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>0.30299999999999999</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>1.1066</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>0.40079999999999999</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>0.8024</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>0.50149999999999995</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>0.50049999999999994</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>0.70140000000000002</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>9.9900000000000003E-2</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>1.0091000000000001</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>4.5</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>1.5385</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>3.5373000000000001</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>2.1198000000000001</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>0.82040000000000002</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>2.0017999999999998</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>0.27200000000000002</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>7.5023</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>1.617</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>3.4247000000000001</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>1.6878</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>2.3729</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>0.33279999999999998</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>3.8494000000000002</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>5.9737999999999998</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>1.4107000000000001</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>1.323</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>2.7711999999999999</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>6.4814999999999996</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>1.0853999999999999</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>2.4443999999999999</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>1.3187</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>1.1887000000000001</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>1.4815</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>0.81299999999999994</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>6.0743999999999998</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>0.57969999999999999</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>0.5091</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>7.3899999999999993E-2</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>1.0479000000000001</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>2.0863999999999998</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>3.8319999999999999</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>1.5107999999999999</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>3.5714000000000001</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>0.65500000000000003</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>6.2222</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>4.2988</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>0.20530000000000001</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>0.4158</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>4.5069999999999997</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>1.6249</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>0.97219999999999995</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>0.83330000000000004</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>0.71020000000000005</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>0.99080000000000001</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>1.0057</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>0.36080000000000001</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>0.1464</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>0.22470000000000001</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>0.83650000000000002</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>3.0255999999999998</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>1.8809</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>3.2557999999999998</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>0.52629999999999999</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>1.1673</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>9.2456999999999994</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>1.7202999999999999</c:v>
-                </c:pt>
-                <c:pt idx="185">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="186">
-                  <c:v>2.5095000000000001</c:v>
-                </c:pt>
-                <c:pt idx="187">
-                  <c:v>0.15140000000000001</c:v>
-                </c:pt>
-                <c:pt idx="188">
-                  <c:v>1.3720000000000001</c:v>
-                </c:pt>
-                <c:pt idx="189">
-                  <c:v>1.0078</c:v>
-                </c:pt>
-                <c:pt idx="190">
-                  <c:v>1.8987000000000001</c:v>
-                </c:pt>
-                <c:pt idx="191">
-                  <c:v>4.0221</c:v>
-                </c:pt>
-                <c:pt idx="192">
-                  <c:v>1.7627999999999999</c:v>
-                </c:pt>
-                <c:pt idx="193">
-                  <c:v>1.7670999999999999</c:v>
-                </c:pt>
-                <c:pt idx="194">
-                  <c:v>4.2755000000000001</c:v>
-                </c:pt>
-                <c:pt idx="195">
-                  <c:v>0.60880000000000001</c:v>
-                </c:pt>
-                <c:pt idx="196">
-                  <c:v>0.45490000000000003</c:v>
-                </c:pt>
-                <c:pt idx="197">
-                  <c:v>0.60609999999999997</c:v>
-                </c:pt>
-                <c:pt idx="198">
-                  <c:v>0.3876</c:v>
-                </c:pt>
-                <c:pt idx="199">
-                  <c:v>2.0537000000000001</c:v>
-                </c:pt>
-                <c:pt idx="200">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="201">
-                  <c:v>4.5118999999999998</c:v>
-                </c:pt>
-                <c:pt idx="202">
-                  <c:v>0.96079999999999999</c:v>
-                </c:pt>
-                <c:pt idx="203">
-                  <c:v>2.1635</c:v>
-                </c:pt>
-                <c:pt idx="204">
-                  <c:v>3.0158999999999998</c:v>
-                </c:pt>
-                <c:pt idx="205">
-                  <c:v>2.0095999999999998</c:v>
-                </c:pt>
-                <c:pt idx="206">
-                  <c:v>0.70920000000000005</c:v>
-                </c:pt>
-                <c:pt idx="207">
-                  <c:v>0.55640000000000001</c:v>
-                </c:pt>
-                <c:pt idx="208">
-                  <c:v>0.63690000000000002</c:v>
-                </c:pt>
-                <c:pt idx="209">
-                  <c:v>0.56499999999999995</c:v>
-                </c:pt>
-                <c:pt idx="210">
-                  <c:v>0.81299999999999994</c:v>
-                </c:pt>
-                <c:pt idx="211">
-                  <c:v>1.6393</c:v>
-                </c:pt>
-                <c:pt idx="212">
-                  <c:v>0.16220000000000001</c:v>
-                </c:pt>
-                <c:pt idx="213">
-                  <c:v>2.0747</c:v>
-                </c:pt>
-                <c:pt idx="214">
-                  <c:v>5.1597</c:v>
-                </c:pt>
-                <c:pt idx="215">
-                  <c:v>0.87790000000000001</c:v>
-                </c:pt>
-                <c:pt idx="216">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="217">
-                  <c:v>2.4691000000000001</c:v>
-                </c:pt>
-                <c:pt idx="218">
-                  <c:v>0.89870000000000005</c:v>
-                </c:pt>
-                <c:pt idx="219">
-                  <c:v>0.48859999999999998</c:v>
-                </c:pt>
-                <c:pt idx="220">
-                  <c:v>0.1653</c:v>
-                </c:pt>
-                <c:pt idx="221">
-                  <c:v>3.2071999999999998</c:v>
-                </c:pt>
-                <c:pt idx="222">
-                  <c:v>2.0160999999999998</c:v>
-                </c:pt>
-                <c:pt idx="223">
-                  <c:v>0.48120000000000002</c:v>
-                </c:pt>
-                <c:pt idx="224">
-                  <c:v>1.3622000000000001</c:v>
-                </c:pt>
-                <c:pt idx="225">
-                  <c:v>0.31900000000000001</c:v>
-                </c:pt>
-                <c:pt idx="226">
-                  <c:v>3.0644999999999998</c:v>
-                </c:pt>
-                <c:pt idx="227">
-                  <c:v>3.6892</c:v>
-                </c:pt>
-                <c:pt idx="228">
-                  <c:v>1.3656999999999999</c:v>
-                </c:pt>
-                <c:pt idx="229">
-                  <c:v>2.4775</c:v>
-                </c:pt>
-                <c:pt idx="230">
-                  <c:v>2.8782000000000001</c:v>
-                </c:pt>
-                <c:pt idx="231">
-                  <c:v>0.43259999999999998</c:v>
-                </c:pt>
-                <c:pt idx="232">
-                  <c:v>1.7316</c:v>
-                </c:pt>
-                <c:pt idx="233">
-                  <c:v>7.2499999999999995E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:axId val="111268608"/>
-        <c:axId val="111271296"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="111268608"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:majorGridlines/>
-        <c:minorGridlines/>
-        <c:title>
-          <c:layout/>
-        </c:title>
-        <c:numFmt formatCode="0.0_ " sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111271296"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="111271296"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:minorGridlines/>
-        <c:title>
-          <c:layout/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6350"/>
-        </c:spPr>
-        <c:crossAx val="111268608"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -5299,10 +4187,10 @@
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>117</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5316,36 +4204,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>128</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>163</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5493,7 +4351,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -9790,8 +8648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B129" sqref="B129"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="P113" sqref="P113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -11961,15 +10819,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -11988,8 +10846,20 @@
       <c r="G1" s="4">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="4">
+        <v>3</v>
+      </c>
+      <c r="I1" s="4">
+        <v>-0.3</v>
+      </c>
+      <c r="J1" s="4">
+        <v>-7.2</v>
+      </c>
+      <c r="K1" s="4">
+        <v>-2.9329999999999998</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="C2" s="4">
         <v>-2.9</v>
       </c>
@@ -12005,8 +10875,20 @@
       <c r="G2" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" s="4">
+        <v>1</v>
+      </c>
+      <c r="I2" s="4">
+        <v>-5.6</v>
+      </c>
+      <c r="J2" s="4">
+        <v>-5.6</v>
+      </c>
+      <c r="K2" s="4">
+        <v>-5.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="C3" s="4">
         <v>-2.8</v>
       </c>
@@ -12022,8 +10904,20 @@
       <c r="G3" s="4">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" s="4">
+        <v>1</v>
+      </c>
+      <c r="I3" s="4">
+        <v>-3.5</v>
+      </c>
+      <c r="J3" s="4">
+        <v>-3.5</v>
+      </c>
+      <c r="K3" s="4">
+        <v>-3.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="C4" s="4">
         <v>-2.7</v>
       </c>
@@ -12039,8 +10933,20 @@
       <c r="G4" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" s="4">
+        <v>3</v>
+      </c>
+      <c r="I4" s="4">
+        <v>-0.3</v>
+      </c>
+      <c r="J4" s="4">
+        <v>-5.0999999999999996</v>
+      </c>
+      <c r="K4" s="4">
+        <v>-2.367</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="C5" s="4">
         <v>-2.6</v>
       </c>
@@ -12056,8 +10962,20 @@
       <c r="G5" s="4">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5" s="4">
+        <v>3</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4">
+        <v>-2.1</v>
+      </c>
+      <c r="K5" s="4">
+        <v>-0.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="C6" s="4">
         <v>-2.5</v>
       </c>
@@ -12073,8 +10991,20 @@
       <c r="G6" s="4">
         <v>4.28</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" s="4">
+        <v>5</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0</v>
+      </c>
+      <c r="J6" s="4">
+        <v>-3.7</v>
+      </c>
+      <c r="K6" s="4">
+        <v>-1.44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="C7" s="4">
         <v>-2.4</v>
       </c>
@@ -12090,8 +11020,20 @@
       <c r="G7" s="4">
         <v>4.28</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7" s="4">
+        <v>5</v>
+      </c>
+      <c r="I7" s="4">
+        <v>-0.1</v>
+      </c>
+      <c r="J7" s="4">
+        <v>-1.8</v>
+      </c>
+      <c r="K7" s="4">
+        <v>-0.98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="C8" s="4">
         <v>-2.2999999999999998</v>
       </c>
@@ -12107,8 +11049,20 @@
       <c r="G8" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8" s="4">
+        <v>2</v>
+      </c>
+      <c r="I8" s="4">
+        <v>-0.6</v>
+      </c>
+      <c r="J8" s="4">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="K8" s="4">
+        <v>-0.85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="C9" s="4">
         <v>-2.2000000000000002</v>
       </c>
@@ -12124,8 +11078,20 @@
       <c r="G9" s="4">
         <v>3.7370000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9" s="4">
+        <v>8</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4">
+        <v>-7.3</v>
+      </c>
+      <c r="K9" s="4">
+        <v>-1.5629999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="C10" s="4">
         <v>-2.1</v>
       </c>
@@ -12141,8 +11107,20 @@
       <c r="G10" s="4">
         <v>1.56</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10" s="4">
+        <v>5</v>
+      </c>
+      <c r="I10" s="4">
+        <v>-1</v>
+      </c>
+      <c r="J10" s="4">
+        <v>-8</v>
+      </c>
+      <c r="K10" s="4">
+        <v>-4.12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="C11" s="4">
         <v>-2</v>
       </c>
@@ -12158,8 +11136,20 @@
       <c r="G11" s="4">
         <v>2.8079999999999998</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11" s="4">
+        <v>12</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0</v>
+      </c>
+      <c r="J11" s="4">
+        <v>-7.2</v>
+      </c>
+      <c r="K11" s="4">
+        <v>-2.2669999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="C12" s="4">
         <v>-1.9</v>
       </c>
@@ -12175,8 +11165,20 @@
       <c r="G12" s="4">
         <v>1.333</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12" s="4">
+        <v>6</v>
+      </c>
+      <c r="I12" s="4">
+        <v>-1.4</v>
+      </c>
+      <c r="J12" s="4">
+        <v>-6</v>
+      </c>
+      <c r="K12" s="4">
+        <v>-2.4500000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="C13" s="4">
         <v>-1.8</v>
       </c>
@@ -12192,8 +11194,20 @@
       <c r="G13" s="4">
         <v>1.857</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="H13" s="4">
+        <v>7</v>
+      </c>
+      <c r="I13" s="4">
+        <v>-0.1</v>
+      </c>
+      <c r="J13" s="4">
+        <v>-3.4</v>
+      </c>
+      <c r="K13" s="4">
+        <v>-1.871</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="C14" s="4">
         <v>-1.7</v>
       </c>
@@ -12209,8 +11223,20 @@
       <c r="G14" s="4">
         <v>2.3620000000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="H14" s="4">
+        <v>13</v>
+      </c>
+      <c r="I14" s="4">
+        <v>-0.4</v>
+      </c>
+      <c r="J14" s="4">
+        <v>-5.3</v>
+      </c>
+      <c r="K14" s="4">
+        <v>-1.6619999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="C15" s="4">
         <v>-1.6</v>
       </c>
@@ -12226,8 +11252,20 @@
       <c r="G15" s="4">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="H15" s="4">
+        <v>11</v>
+      </c>
+      <c r="I15" s="4">
+        <v>-0.2</v>
+      </c>
+      <c r="J15" s="4">
+        <v>-4.5999999999999996</v>
+      </c>
+      <c r="K15" s="4">
+        <v>-1.6910000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="C16" s="4">
         <v>-1.5</v>
       </c>
@@ -12243,8 +11281,20 @@
       <c r="G16" s="4">
         <v>2.2530000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="3:7">
+      <c r="H16" s="4">
+        <v>15</v>
+      </c>
+      <c r="I16" s="4">
+        <v>0</v>
+      </c>
+      <c r="J16" s="4">
+        <v>-4.9000000000000004</v>
+      </c>
+      <c r="K16" s="4">
+        <v>-1.653</v>
+      </c>
+    </row>
+    <row r="17" spans="3:11">
       <c r="C17" s="4">
         <v>-1.4</v>
       </c>
@@ -12260,8 +11310,20 @@
       <c r="G17" s="4">
         <v>2.2930000000000001</v>
       </c>
-    </row>
-    <row r="18" spans="3:7">
+      <c r="H17" s="4">
+        <v>15</v>
+      </c>
+      <c r="I17" s="4">
+        <v>-0.2</v>
+      </c>
+      <c r="J17" s="4">
+        <v>-5.6</v>
+      </c>
+      <c r="K17" s="4">
+        <v>-2.2069999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="3:11">
       <c r="C18" s="4">
         <v>-1.3</v>
       </c>
@@ -12277,8 +11339,20 @@
       <c r="G18" s="4">
         <v>1.4239999999999999</v>
       </c>
-    </row>
-    <row r="19" spans="3:7">
+      <c r="H18" s="4">
+        <v>25</v>
+      </c>
+      <c r="I18" s="4">
+        <v>0</v>
+      </c>
+      <c r="J18" s="4">
+        <v>-5.5</v>
+      </c>
+      <c r="K18" s="4">
+        <v>-2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11">
       <c r="C19" s="4">
         <v>-1.2</v>
       </c>
@@ -12294,8 +11368,20 @@
       <c r="G19" s="4">
         <v>2.1629999999999998</v>
       </c>
-    </row>
-    <row r="20" spans="3:7">
+      <c r="H19" s="4">
+        <v>16</v>
+      </c>
+      <c r="I19" s="4">
+        <v>0</v>
+      </c>
+      <c r="J19" s="4">
+        <v>-5</v>
+      </c>
+      <c r="K19" s="4">
+        <v>-1.419</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11">
       <c r="C20" s="4">
         <v>-1.1000000000000001</v>
       </c>
@@ -12311,8 +11397,20 @@
       <c r="G20" s="4">
         <v>2.8540000000000001</v>
       </c>
-    </row>
-    <row r="21" spans="3:7">
+      <c r="H20" s="4">
+        <v>28</v>
+      </c>
+      <c r="I20" s="4">
+        <v>0</v>
+      </c>
+      <c r="J20" s="4">
+        <v>-4.3</v>
+      </c>
+      <c r="K20" s="4">
+        <v>-1.464</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11">
       <c r="C21" s="4">
         <v>-1</v>
       </c>
@@ -12328,8 +11426,20 @@
       <c r="G21" s="4">
         <v>2.371</v>
       </c>
-    </row>
-    <row r="22" spans="3:7">
+      <c r="H21" s="4">
+        <v>17</v>
+      </c>
+      <c r="I21" s="4">
+        <v>0</v>
+      </c>
+      <c r="J21" s="4">
+        <v>-5.4</v>
+      </c>
+      <c r="K21" s="4">
+        <v>-1.7529999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11">
       <c r="C22" s="4">
         <v>-0.9</v>
       </c>
@@ -12345,8 +11455,20 @@
       <c r="G22" s="4">
         <v>1.5680000000000001</v>
       </c>
-    </row>
-    <row r="23" spans="3:7">
+      <c r="H22" s="4">
+        <v>38</v>
+      </c>
+      <c r="I22" s="4">
+        <v>0</v>
+      </c>
+      <c r="J22" s="4">
+        <v>-9.1999999999999993</v>
+      </c>
+      <c r="K22" s="4">
+        <v>-1.911</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11">
       <c r="C23" s="4">
         <v>-0.8</v>
       </c>
@@ -12362,8 +11484,20 @@
       <c r="G23" s="4">
         <v>1.621</v>
       </c>
-    </row>
-    <row r="24" spans="3:7">
+      <c r="H23" s="4">
+        <v>53</v>
+      </c>
+      <c r="I23" s="4">
+        <v>0</v>
+      </c>
+      <c r="J23" s="4">
+        <v>-4.8</v>
+      </c>
+      <c r="K23" s="4">
+        <v>-1.3420000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11">
       <c r="C24" s="4">
         <v>-0.7</v>
       </c>
@@ -12379,8 +11513,20 @@
       <c r="G24" s="4">
         <v>2.2559999999999998</v>
       </c>
-    </row>
-    <row r="25" spans="3:7">
+      <c r="H24" s="4">
+        <v>57</v>
+      </c>
+      <c r="I24" s="4">
+        <v>0</v>
+      </c>
+      <c r="J24" s="4">
+        <v>-8.1999999999999993</v>
+      </c>
+      <c r="K24" s="4">
+        <v>-1.4159999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11">
       <c r="C25" s="4">
         <v>-0.6</v>
       </c>
@@ -12396,8 +11542,20 @@
       <c r="G25" s="4">
         <v>1.6020000000000001</v>
       </c>
-    </row>
-    <row r="26" spans="3:7">
+      <c r="H25" s="4">
+        <v>47</v>
+      </c>
+      <c r="I25" s="4">
+        <v>0</v>
+      </c>
+      <c r="J25" s="4">
+        <v>-6.3</v>
+      </c>
+      <c r="K25" s="4">
+        <v>-1.5740000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11">
       <c r="C26" s="4">
         <v>-0.5</v>
       </c>
@@ -12413,8 +11571,20 @@
       <c r="G26" s="4">
         <v>1.53</v>
       </c>
-    </row>
-    <row r="27" spans="3:7">
+      <c r="H26" s="4">
+        <v>70</v>
+      </c>
+      <c r="I26" s="4">
+        <v>0</v>
+      </c>
+      <c r="J26" s="4">
+        <v>-8.9</v>
+      </c>
+      <c r="K26" s="4">
+        <v>-1.679</v>
+      </c>
+    </row>
+    <row r="27" spans="3:11">
       <c r="C27" s="4">
         <v>-0.4</v>
       </c>
@@ -12430,8 +11600,20 @@
       <c r="G27" s="4">
         <v>1.52</v>
       </c>
-    </row>
-    <row r="28" spans="3:7">
+      <c r="H27" s="4">
+        <v>96</v>
+      </c>
+      <c r="I27" s="4">
+        <v>0</v>
+      </c>
+      <c r="J27" s="4">
+        <v>-5.3</v>
+      </c>
+      <c r="K27" s="4">
+        <v>-1.306</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11">
       <c r="C28" s="4">
         <v>-0.3</v>
       </c>
@@ -12447,8 +11629,20 @@
       <c r="G28" s="4">
         <v>1.5409999999999999</v>
       </c>
-    </row>
-    <row r="29" spans="3:7">
+      <c r="H28" s="4">
+        <v>91</v>
+      </c>
+      <c r="I28" s="4">
+        <v>0</v>
+      </c>
+      <c r="J28" s="4">
+        <v>-4.5999999999999996</v>
+      </c>
+      <c r="K28" s="4">
+        <v>-1.3560000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="3:11">
       <c r="C29" s="4">
         <v>-0.2</v>
       </c>
@@ -12464,8 +11658,20 @@
       <c r="G29" s="4">
         <v>1.357</v>
       </c>
-    </row>
-    <row r="30" spans="3:7">
+      <c r="H29" s="4">
+        <v>249</v>
+      </c>
+      <c r="I29" s="4">
+        <v>0</v>
+      </c>
+      <c r="J29" s="4">
+        <v>-8.8000000000000007</v>
+      </c>
+      <c r="K29" s="4">
+        <v>-1.343</v>
+      </c>
+    </row>
+    <row r="30" spans="3:11">
       <c r="C30" s="4">
         <v>-0.1</v>
       </c>
@@ -12481,8 +11687,20 @@
       <c r="G30" s="4">
         <v>1.498</v>
       </c>
-    </row>
-    <row r="31" spans="3:7">
+      <c r="H30" s="4">
+        <v>112</v>
+      </c>
+      <c r="I30" s="4">
+        <v>0</v>
+      </c>
+      <c r="J30" s="4">
+        <v>-9.9</v>
+      </c>
+      <c r="K30" s="4">
+        <v>-1.5760000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="3:11">
       <c r="C31" s="4">
         <v>0</v>
       </c>
@@ -12498,8 +11716,20 @@
       <c r="G31" s="4">
         <v>1.4390000000000001</v>
       </c>
-    </row>
-    <row r="32" spans="3:7">
+      <c r="H31" s="4">
+        <v>594</v>
+      </c>
+      <c r="I31" s="4">
+        <v>0</v>
+      </c>
+      <c r="J31" s="4">
+        <v>-5.4</v>
+      </c>
+      <c r="K31" s="4">
+        <v>-1.286</v>
+      </c>
+    </row>
+    <row r="32" spans="3:11">
       <c r="C32" s="4">
         <v>0.1</v>
       </c>
@@ -12515,8 +11745,20 @@
       <c r="G32" s="4">
         <v>1.8220000000000001</v>
       </c>
-    </row>
-    <row r="33" spans="3:7">
+      <c r="H32" s="4">
+        <v>122</v>
+      </c>
+      <c r="I32" s="4">
+        <v>0</v>
+      </c>
+      <c r="J32" s="4">
+        <v>-7.1</v>
+      </c>
+      <c r="K32" s="4">
+        <v>-1.2869999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="3:11">
       <c r="C33" s="4">
         <v>0.2</v>
       </c>
@@ -12532,8 +11774,20 @@
       <c r="G33" s="4">
         <v>1.591</v>
       </c>
-    </row>
-    <row r="34" spans="3:7">
+      <c r="H33" s="4">
+        <v>232</v>
+      </c>
+      <c r="I33" s="4">
+        <v>0</v>
+      </c>
+      <c r="J33" s="4">
+        <v>-6.6</v>
+      </c>
+      <c r="K33" s="4">
+        <v>-1.238</v>
+      </c>
+    </row>
+    <row r="34" spans="3:11">
       <c r="C34" s="4">
         <v>0.3</v>
       </c>
@@ -12549,8 +11803,20 @@
       <c r="G34" s="4">
         <v>1.6870000000000001</v>
       </c>
-    </row>
-    <row r="35" spans="3:7">
+      <c r="H34" s="4">
+        <v>105</v>
+      </c>
+      <c r="I34" s="4">
+        <v>0</v>
+      </c>
+      <c r="J34" s="4">
+        <v>-3.8</v>
+      </c>
+      <c r="K34" s="4">
+        <v>-1.163</v>
+      </c>
+    </row>
+    <row r="35" spans="3:11">
       <c r="C35" s="4">
         <v>0.4</v>
       </c>
@@ -12566,8 +11832,20 @@
       <c r="G35" s="4">
         <v>1.6379999999999999</v>
       </c>
-    </row>
-    <row r="36" spans="3:7">
+      <c r="H35" s="4">
+        <v>92</v>
+      </c>
+      <c r="I35" s="4">
+        <v>0</v>
+      </c>
+      <c r="J35" s="4">
+        <v>-5.6</v>
+      </c>
+      <c r="K35" s="4">
+        <v>-1.236</v>
+      </c>
+    </row>
+    <row r="36" spans="3:11">
       <c r="C36" s="4">
         <v>0.5</v>
       </c>
@@ -12583,8 +11861,20 @@
       <c r="G36" s="4">
         <v>1.98</v>
       </c>
-    </row>
-    <row r="37" spans="3:7">
+      <c r="H36" s="4">
+        <v>82</v>
+      </c>
+      <c r="I36" s="4">
+        <v>0</v>
+      </c>
+      <c r="J36" s="4">
+        <v>-4.9000000000000004</v>
+      </c>
+      <c r="K36" s="4">
+        <v>-1.3959999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="3:11">
       <c r="C37" s="4">
         <v>0.6</v>
       </c>
@@ -12600,8 +11890,20 @@
       <c r="G37" s="4">
         <v>1.8779999999999999</v>
       </c>
-    </row>
-    <row r="38" spans="3:7">
+      <c r="H37" s="4">
+        <v>69</v>
+      </c>
+      <c r="I37" s="4">
+        <v>0</v>
+      </c>
+      <c r="J37" s="4">
+        <v>-10.5</v>
+      </c>
+      <c r="K37" s="4">
+        <v>-1.8480000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="3:11">
       <c r="C38" s="4">
         <v>0.7</v>
       </c>
@@ -12617,8 +11919,20 @@
       <c r="G38" s="4">
         <v>1.718</v>
       </c>
-    </row>
-    <row r="39" spans="3:7">
+      <c r="H38" s="4">
+        <v>50</v>
+      </c>
+      <c r="I38" s="4">
+        <v>0</v>
+      </c>
+      <c r="J38" s="4">
+        <v>-10</v>
+      </c>
+      <c r="K38" s="4">
+        <v>-1.6359999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="3:11">
       <c r="C39" s="4">
         <v>0.8</v>
       </c>
@@ -12634,8 +11948,20 @@
       <c r="G39" s="4">
         <v>1.6830000000000001</v>
       </c>
-    </row>
-    <row r="40" spans="3:7">
+      <c r="H39" s="4">
+        <v>35</v>
+      </c>
+      <c r="I39" s="4">
+        <v>0</v>
+      </c>
+      <c r="J39" s="4">
+        <v>-5.6</v>
+      </c>
+      <c r="K39" s="4">
+        <v>-1.6140000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="3:11">
       <c r="C40" s="4">
         <v>0.9</v>
       </c>
@@ -12651,8 +11977,20 @@
       <c r="G40" s="4">
         <v>1.581</v>
       </c>
-    </row>
-    <row r="41" spans="3:7">
+      <c r="H40" s="4">
+        <v>31</v>
+      </c>
+      <c r="I40" s="4">
+        <v>0</v>
+      </c>
+      <c r="J40" s="4">
+        <v>-5.8</v>
+      </c>
+      <c r="K40" s="4">
+        <v>-1.8</v>
+      </c>
+    </row>
+    <row r="41" spans="3:11">
       <c r="C41" s="4">
         <v>1</v>
       </c>
@@ -12668,8 +12006,20 @@
       <c r="G41" s="4">
         <v>2.0099999999999998</v>
       </c>
-    </row>
-    <row r="42" spans="3:7">
+      <c r="H41" s="4">
+        <v>21</v>
+      </c>
+      <c r="I41" s="4">
+        <v>0</v>
+      </c>
+      <c r="J41" s="4">
+        <v>-7.5</v>
+      </c>
+      <c r="K41" s="4">
+        <v>-1.69</v>
+      </c>
+    </row>
+    <row r="42" spans="3:11">
       <c r="C42" s="4">
         <v>1.1000000000000001</v>
       </c>
@@ -12685,8 +12035,20 @@
       <c r="G42" s="4">
         <v>2.02</v>
       </c>
-    </row>
-    <row r="43" spans="3:7">
+      <c r="H42" s="4">
+        <v>20</v>
+      </c>
+      <c r="I42" s="4">
+        <v>0</v>
+      </c>
+      <c r="J42" s="4">
+        <v>-4.0999999999999996</v>
+      </c>
+      <c r="K42" s="4">
+        <v>-1.47</v>
+      </c>
+    </row>
+    <row r="43" spans="3:11">
       <c r="C43" s="4">
         <v>1.2</v>
       </c>
@@ -12702,8 +12064,20 @@
       <c r="G43" s="4">
         <v>2.1139999999999999</v>
       </c>
-    </row>
-    <row r="44" spans="3:7">
+      <c r="H43" s="4">
+        <v>14</v>
+      </c>
+      <c r="I43" s="4">
+        <v>-0.4</v>
+      </c>
+      <c r="J43" s="4">
+        <v>-5.2</v>
+      </c>
+      <c r="K43" s="4">
+        <v>-2.1859999999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="3:11">
       <c r="C44" s="4">
         <v>1.3</v>
       </c>
@@ -12719,8 +12093,20 @@
       <c r="G44" s="4">
         <v>1.7390000000000001</v>
       </c>
-    </row>
-    <row r="45" spans="3:7">
+      <c r="H44" s="4">
+        <v>18</v>
+      </c>
+      <c r="I44" s="4">
+        <v>0</v>
+      </c>
+      <c r="J44" s="4">
+        <v>-7.2</v>
+      </c>
+      <c r="K44" s="4">
+        <v>-1.744</v>
+      </c>
+    </row>
+    <row r="45" spans="3:11">
       <c r="C45" s="4">
         <v>1.4</v>
       </c>
@@ -12736,8 +12122,20 @@
       <c r="G45" s="4">
         <v>2.7210000000000001</v>
       </c>
-    </row>
-    <row r="46" spans="3:7">
+      <c r="H45" s="4">
+        <v>14</v>
+      </c>
+      <c r="I45" s="4">
+        <v>0</v>
+      </c>
+      <c r="J45" s="4">
+        <v>-4.5999999999999996</v>
+      </c>
+      <c r="K45" s="4">
+        <v>-1.8069999999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="3:11">
       <c r="C46" s="4">
         <v>1.5</v>
       </c>
@@ -12753,8 +12151,20 @@
       <c r="G46" s="4">
         <v>3.512</v>
       </c>
-    </row>
-    <row r="47" spans="3:7">
+      <c r="H46" s="4">
+        <v>8</v>
+      </c>
+      <c r="I46" s="4">
+        <v>0</v>
+      </c>
+      <c r="J46" s="4">
+        <v>-3.6</v>
+      </c>
+      <c r="K46" s="4">
+        <v>-1.2130000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="3:11">
       <c r="C47" s="4">
         <v>1.6</v>
       </c>
@@ -12770,8 +12180,20 @@
       <c r="G47" s="4">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="48" spans="3:7">
+      <c r="H47" s="4">
+        <v>5</v>
+      </c>
+      <c r="I47" s="4">
+        <v>-0.3</v>
+      </c>
+      <c r="J47" s="4">
+        <v>-2.2999999999999998</v>
+      </c>
+      <c r="K47" s="4">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="48" spans="3:11">
       <c r="C48" s="4">
         <v>1.7</v>
       </c>
@@ -12787,8 +12209,20 @@
       <c r="G48" s="4">
         <v>2.4670000000000001</v>
       </c>
-    </row>
-    <row r="49" spans="3:7">
+      <c r="H48" s="4">
+        <v>3</v>
+      </c>
+      <c r="I48" s="4">
+        <v>-0.1</v>
+      </c>
+      <c r="J48" s="4">
+        <v>-11.4</v>
+      </c>
+      <c r="K48" s="4">
+        <v>-4.1669999999999998</v>
+      </c>
+    </row>
+    <row r="49" spans="3:11">
       <c r="C49" s="4">
         <v>1.8</v>
       </c>
@@ -12804,8 +12238,20 @@
       <c r="G49" s="4">
         <v>1.7330000000000001</v>
       </c>
-    </row>
-    <row r="50" spans="3:7">
+      <c r="H49" s="4">
+        <v>6</v>
+      </c>
+      <c r="I49" s="4">
+        <v>-0.1</v>
+      </c>
+      <c r="J49" s="4">
+        <v>-4.3</v>
+      </c>
+      <c r="K49" s="4">
+        <v>-1.9830000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="3:11">
       <c r="C50" s="4">
         <v>1.9</v>
       </c>
@@ -12821,8 +12267,20 @@
       <c r="G50" s="4">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="51" spans="3:7">
+      <c r="H50" s="4">
+        <v>8</v>
+      </c>
+      <c r="I50" s="4">
+        <v>0</v>
+      </c>
+      <c r="J50" s="4">
+        <v>-7.2</v>
+      </c>
+      <c r="K50" s="4">
+        <v>-2.2629999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="3:11">
       <c r="C51" s="4">
         <v>2</v>
       </c>
@@ -12838,8 +12296,20 @@
       <c r="G51" s="4">
         <v>2.44</v>
       </c>
-    </row>
-    <row r="52" spans="3:7">
+      <c r="H51" s="4">
+        <v>5</v>
+      </c>
+      <c r="I51" s="4">
+        <v>0</v>
+      </c>
+      <c r="J51" s="4">
+        <v>-8.1</v>
+      </c>
+      <c r="K51" s="4">
+        <v>-2.72</v>
+      </c>
+    </row>
+    <row r="52" spans="3:11">
       <c r="C52" s="4">
         <v>2.1</v>
       </c>
@@ -12855,8 +12325,20 @@
       <c r="G52" s="4">
         <v>1.6830000000000001</v>
       </c>
-    </row>
-    <row r="53" spans="3:7">
+      <c r="H52" s="4">
+        <v>6</v>
+      </c>
+      <c r="I52" s="4">
+        <v>-0.9</v>
+      </c>
+      <c r="J52" s="4">
+        <v>-3.2</v>
+      </c>
+      <c r="K52" s="4">
+        <v>-1.833</v>
+      </c>
+    </row>
+    <row r="53" spans="3:11">
       <c r="C53" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -12872,8 +12354,20 @@
       <c r="G53" s="4">
         <v>3.2330000000000001</v>
       </c>
-    </row>
-    <row r="54" spans="3:7">
+      <c r="H53" s="4">
+        <v>3</v>
+      </c>
+      <c r="I53" s="4">
+        <v>0</v>
+      </c>
+      <c r="J53" s="4">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="K53" s="4">
+        <v>-0.9</v>
+      </c>
+    </row>
+    <row r="54" spans="3:11">
       <c r="C54" s="4">
         <v>2.2999999999999998</v>
       </c>
@@ -12889,8 +12383,20 @@
       <c r="G54" s="4">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="55" spans="3:7">
+      <c r="H54" s="4">
+        <v>4</v>
+      </c>
+      <c r="I54" s="4">
+        <v>-0.4</v>
+      </c>
+      <c r="J54" s="4">
+        <v>-4.5</v>
+      </c>
+      <c r="K54" s="4">
+        <v>-2.4750000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="3:11">
       <c r="C55" s="4">
         <v>2.4</v>
       </c>
@@ -12906,8 +12412,20 @@
       <c r="G55" s="4">
         <v>1.4750000000000001</v>
       </c>
-    </row>
-    <row r="56" spans="3:7">
+      <c r="H55" s="4">
+        <v>4</v>
+      </c>
+      <c r="I55" s="4">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="J55" s="4">
+        <v>-8.4</v>
+      </c>
+      <c r="K55" s="4">
+        <v>-4.4749999999999996</v>
+      </c>
+    </row>
+    <row r="56" spans="3:11">
       <c r="C56" s="4">
         <v>2.5</v>
       </c>
@@ -12923,8 +12441,20 @@
       <c r="G56" s="4">
         <v>6.05</v>
       </c>
-    </row>
-    <row r="57" spans="3:7">
+      <c r="H56" s="4">
+        <v>2</v>
+      </c>
+      <c r="I56" s="4">
+        <v>-0.2</v>
+      </c>
+      <c r="J56" s="4">
+        <v>-1.2</v>
+      </c>
+      <c r="K56" s="4">
+        <v>-0.7</v>
+      </c>
+    </row>
+    <row r="57" spans="3:11">
       <c r="C57" s="4">
         <v>2.6</v>
       </c>
@@ -12940,8 +12470,20 @@
       <c r="G57" s="4">
         <v>2.7330000000000001</v>
       </c>
-    </row>
-    <row r="58" spans="3:7">
+      <c r="H57" s="4">
+        <v>3</v>
+      </c>
+      <c r="I57" s="4">
+        <v>-0.6</v>
+      </c>
+      <c r="J57" s="4">
+        <v>-4.7</v>
+      </c>
+      <c r="K57" s="4">
+        <v>-2.8</v>
+      </c>
+    </row>
+    <row r="58" spans="3:11">
       <c r="C58" s="4">
         <v>2.7</v>
       </c>
@@ -12957,8 +12499,20 @@
       <c r="G58" s="4">
         <v>3.2</v>
       </c>
-    </row>
-    <row r="59" spans="3:7">
+      <c r="H58" s="4">
+        <v>1</v>
+      </c>
+      <c r="I58" s="4">
+        <v>-3.2</v>
+      </c>
+      <c r="J58" s="4">
+        <v>-3.2</v>
+      </c>
+      <c r="K58" s="4">
+        <v>-3.2</v>
+      </c>
+    </row>
+    <row r="59" spans="3:11">
       <c r="C59" s="4">
         <v>2.8</v>
       </c>
@@ -12974,8 +12528,20 @@
       <c r="G59" s="4">
         <v>3.0329999999999999</v>
       </c>
-    </row>
-    <row r="60" spans="3:7">
+      <c r="H59" s="4">
+        <v>3</v>
+      </c>
+      <c r="I59" s="4">
+        <v>-1.3</v>
+      </c>
+      <c r="J59" s="4">
+        <v>-6</v>
+      </c>
+      <c r="K59" s="4">
+        <v>-2.9670000000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="3:11">
       <c r="C60" s="4">
         <v>2.9</v>
       </c>
@@ -12990,6 +12556,18 @@
       </c>
       <c r="G60" s="4">
         <v>2.2999999999999998</v>
+      </c>
+      <c r="H60" s="4">
+        <v>1</v>
+      </c>
+      <c r="I60" s="4">
+        <v>-3.8</v>
+      </c>
+      <c r="J60" s="4">
+        <v>-3.8</v>
+      </c>
+      <c r="K60" s="4">
+        <v>-3.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>